<commit_message>
retrieving 2019 lowry numbers
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -197,6 +197,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -280,20 +281,20 @@
   </sheetPr>
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1:G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27"/>
@@ -1237,14 +1238,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="1" sqref="F1:G1 F20"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
martin curve wo ref depth
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2017-fluxes" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="low-N-subtracted" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="protein flux calc" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="martin power law" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="234">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -734,7 +735,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -762,6 +763,21 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -840,7 +856,868 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2017 P1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Organic C flux (mg C/m2/day)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.12177386572676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.32957111802758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.17726210868461</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.18437848409334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>168</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="19493427"/>
+        <c:axId val="86981926"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="19493427"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (mg/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="86981926"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="86981926"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="19493427"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2017 P2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Organic C flux (mg C/m2/day)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$9:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.78334661696259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.03416289552556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.32232450014019</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.828830860507312</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.47769543896914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.96315848404831</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$B$9:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>452</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="63047033"/>
+        <c:axId val="50609425"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="63047033"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (mg C/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50609425"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="50609425"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="63047033"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>218520</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>483840</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>143640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7045200" y="210240"/>
+        <a:ext cx="5955120" cy="4484880"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>288000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>523800</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>124200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7114680" y="4790520"/>
+        <a:ext cx="5925600" cy="5412240"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -850,18 +1727,18 @@
   </sheetPr>
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.63"/>
@@ -1791,7 +2668,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1806,15 +2683,15 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1829,15 +2706,13 @@
   </sheetPr>
   <dimension ref="A1:BJ70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="BD11" activeCellId="0" sqref="BD11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.2"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="60.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13161,10 +14036,172 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.6"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>2.12177386572676</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1.32957111802758</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2.17726210868461</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>5.18437848409334</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>6.78334661696259</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>2.03416289552556</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1.32232450014019</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>265</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.828830860507312</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>365</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>3.47769543896914</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>452</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1.96315848404831</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
calc true 100 m corrected bs
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2017-fluxes" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="237">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -725,6 +725,15 @@
   </si>
   <si>
     <t xml:space="preserve">4-22_69m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fz C flux organic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fz0(z/z0) Normalized to 74 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fz0(z/z0) Normalized to 73 m</t>
   </si>
 </sst>
 </file>
@@ -919,7 +928,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -966,7 +975,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Organic C flux (mg C/m2/day)</c:v>
+                  <c:v>Fz C flux organic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1014,6 +1023,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1032,6 +1042,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1103,11 +1114,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="19493427"/>
-        <c:axId val="86981926"/>
+        <c:axId val="48441071"/>
+        <c:axId val="75061229"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="19493427"/>
+        <c:axId val="48441071"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,7 +1152,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1163,12 +1174,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86981926"/>
+        <c:crossAx val="75061229"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86981926"/>
+        <c:axId val="75061229"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1211,7 +1222,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1233,9 +1244,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19493427"/>
+        <c:crossAx val="48441071"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1281,7 +1292,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1328,7 +1339,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Organic C flux (mg C/m2/day)</c:v>
+                  <c:v>Fz C flux organic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1376,6 +1387,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1394,6 +1406,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1477,11 +1490,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="63047033"/>
-        <c:axId val="50609425"/>
+        <c:axId val="94115925"/>
+        <c:axId val="4004371"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63047033"/>
+        <c:axId val="94115925"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1515,7 +1528,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1537,12 +1550,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50609425"/>
+        <c:crossAx val="4004371"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50609425"/>
+        <c:axId val="4004371"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1585,7 +1598,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1607,9 +1620,749 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63047033"/>
+        <c:crossAx val="94115925"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2017 P1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fz C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.22176805440372</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.32957111802758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.69507659059645</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.01848578146802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.12177386572676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.32957111802758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.17726210868461</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.18437848409334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="66864873"/>
+        <c:axId val="31283442"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="66864873"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (mg/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31283442"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="31283442"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="66864873"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2017 P2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fz C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$D$9:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.92270191494882</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.03416289552556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.12405628133949</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.38428996320923</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.1708144776278</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.595090805172</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$9:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.78334661696259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.03416289552556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.32232450014019</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.828830860507312</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.47769543896914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.96315848404831</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="20032387"/>
+        <c:axId val="62940719"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="20032387"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (mg C/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="62940719"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="62940719"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="20032387"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1659,16 +2412,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>218520</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>444240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>483840</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>68400</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1676,8 +2429,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7045200" y="210240"/>
-        <a:ext cx="5955120" cy="4484880"/>
+        <a:off x="4835160" y="86040"/>
+        <a:ext cx="5322600" cy="4484520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1689,16 +2442,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>464760</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>523800</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>50040</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1706,12 +2459,72 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7114680" y="4790520"/>
-        <a:ext cx="5925600" cy="5412240"/>
+        <a:off x="4855680" y="5411880"/>
+        <a:ext cx="5283720" cy="4818960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>328320</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>766440</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="10417680" y="0"/>
+        <a:ext cx="5322600" cy="4484520"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>294120</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>153000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>693360</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>95400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="10383480" y="5192280"/>
+        <a:ext cx="5283720" cy="4818960"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1727,11 +2540,11 @@
   </sheetPr>
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.04"/>
@@ -2683,11 +3496,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2706,13 +3519,13 @@
   </sheetPr>
   <dimension ref="A1:BJ70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.19"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="60.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14049,13 +14862,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U57" activeCellId="0" sqref="U57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.29"/>
@@ -14070,7 +14883,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>234</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14083,6 +14899,10 @@
       <c r="C2" s="0" t="n">
         <v>2.12177386572676</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">$C$3*(B2/$B$3)</f>
+        <v>1.22176805440372</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -14094,6 +14914,10 @@
       <c r="C3" s="0" t="n">
         <v>1.32957111802758</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">$C$3*(B3/$B$3)</f>
+        <v>1.32957111802758</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -14105,6 +14929,10 @@
       <c r="C4" s="0" t="n">
         <v>2.17726210868461</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">$C$3*(B4/$B$3)</f>
+        <v>2.69507659059645</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -14116,6 +14944,10 @@
       <c r="C5" s="0" t="n">
         <v>5.18437848409334</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">$C$3*(B5/$B$3)</f>
+        <v>3.01848578146802</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -14125,7 +14957,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>9</v>
+        <v>234</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14138,6 +14973,10 @@
       <c r="C9" s="0" t="n">
         <v>6.78334661696259</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">$C$10*(B9/$B$10)</f>
+        <v>1.92270191494882</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -14149,6 +14988,10 @@
       <c r="C10" s="0" t="n">
         <v>2.03416289552556</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">$C$10*(B10/$B$10)</f>
+        <v>2.03416289552556</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -14160,6 +15003,10 @@
       <c r="C11" s="0" t="n">
         <v>1.32232450014019</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">$C$10*(B11/$B$10)</f>
+        <v>4.12405628133949</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -14171,6 +15018,10 @@
       <c r="C12" s="0" t="n">
         <v>0.828830860507312</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">$C$10*(B12/$B$10)</f>
+        <v>7.38428996320923</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -14182,6 +15033,10 @@
       <c r="C13" s="0" t="n">
         <v>3.47769543896914</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">$C$10*(B13/$B$10)</f>
+        <v>10.1708144776278</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -14192,6 +15047,10 @@
       </c>
       <c r="C14" s="0" t="n">
         <v>1.96315848404831</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">$C$10*(B14/$B$10)</f>
+        <v>12.595090805172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed 2017 fluxes csv
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="2017-fluxes" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="2017-fluxes-old" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="low-N-subtracted" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="protein flux calc" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="martin power law" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="2017-fluxes" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="243">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -734,15 +735,34 @@
   </si>
   <si>
     <t xml:space="preserve">fz0(z/z0) Normalized to 73 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure [dbar]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trap type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Org C flux (umol C/m2/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protein flux (ug/m2/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon protein flux (umol C/m2/day)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -831,7 +851,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -853,6 +873,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -928,7 +952,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1114,11 +1138,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48441071"/>
-        <c:axId val="75061229"/>
+        <c:axId val="46082030"/>
+        <c:axId val="86020807"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48441071"/>
+        <c:axId val="46082030"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,12 +1198,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75061229"/>
+        <c:crossAx val="86020807"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75061229"/>
+        <c:axId val="86020807"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1244,7 +1268,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48441071"/>
+        <c:crossAx val="46082030"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1292,7 +1316,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1490,11 +1514,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="94115925"/>
-        <c:axId val="4004371"/>
+        <c:axId val="20189624"/>
+        <c:axId val="6746575"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94115925"/>
+        <c:axId val="20189624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1550,12 +1574,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4004371"/>
+        <c:crossAx val="6746575"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4004371"/>
+        <c:axId val="6746575"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1620,7 +1644,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94115925"/>
+        <c:crossAx val="20189624"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1668,7 +1692,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1854,11 +1878,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="66864873"/>
-        <c:axId val="31283442"/>
+        <c:axId val="84776988"/>
+        <c:axId val="42953855"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66864873"/>
+        <c:axId val="84776988"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1914,12 +1938,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31283442"/>
+        <c:crossAx val="42953855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="31283442"/>
+        <c:axId val="42953855"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1984,7 +2008,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66864873"/>
+        <c:crossAx val="84776988"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2032,7 +2056,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2230,11 +2254,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="20032387"/>
-        <c:axId val="62940719"/>
+        <c:axId val="6896757"/>
+        <c:axId val="22331646"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20032387"/>
+        <c:axId val="6896757"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2290,12 +2314,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62940719"/>
+        <c:crossAx val="22331646"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62940719"/>
+        <c:axId val="22331646"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2360,7 +2384,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20032387"/>
+        <c:crossAx val="6896757"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2419,9 +2443,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>68400</xdr:colOff>
+      <xdr:colOff>68040</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2429,8 +2453,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4835160" y="86040"/>
-        <a:ext cx="5322600" cy="4484520"/>
+        <a:off x="4837680" y="86040"/>
+        <a:ext cx="5331240" cy="4484160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2449,9 +2473,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>50040</xdr:colOff>
+      <xdr:colOff>49680</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2459,8 +2483,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4855680" y="5411880"/>
-        <a:ext cx="5283720" cy="4818960"/>
+        <a:off x="4858200" y="5411880"/>
+        <a:ext cx="5292360" cy="4818600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2479,9 +2503,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>766440</xdr:colOff>
+      <xdr:colOff>766080</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>95040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2489,8 +2513,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10417680" y="0"/>
-        <a:ext cx="5322600" cy="4484520"/>
+        <a:off x="10429200" y="0"/>
+        <a:ext cx="5329800" cy="4484160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2509,9 +2533,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>693360</xdr:colOff>
+      <xdr:colOff>693000</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>95040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2519,8 +2543,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10383480" y="5192280"/>
-        <a:ext cx="5283720" cy="4818960"/>
+        <a:off x="10395000" y="5192280"/>
+        <a:ext cx="5290920" cy="4818600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2541,10 +2565,10 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.04"/>
@@ -3500,7 +3524,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3519,11 +3543,11 @@
   </sheetPr>
   <dimension ref="A1:BJ70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AW5" activeCellId="0" sqref="AW5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.19"/>
   </cols>
@@ -14864,11 +14888,11 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="U57" activeCellId="0" sqref="U57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.29"/>
@@ -15063,4 +15087,1656 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J70"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F70" activeCellId="0" sqref="F70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D2" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>88.65132562</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>190.8767912</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>329.466918726015</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>329.466918726015</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>159.3757707</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>6.80101053224957</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>53.60557055</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>1380.74796747967</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1380.74796747967</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>6.33046700778707</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>127.9433857</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>240.000000011294</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>240.000000011294</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>25.7141237285309</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>45.62906039</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>952.869565217391</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>952.869565217391</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>132.0557482</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>37.4768756857119</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>82.12926293</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>90</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>103.7328318</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>90</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>18.2032700523594</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>55.80971782</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>355</v>
+      </c>
+      <c r="D13" s="6" t="n">
+        <v>355</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>52.10180487</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>601.724877856229</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>601.724877856229</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>355</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <v>355</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>8.48014138257403</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>169.7946237</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>1286.93766937669</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>1286.93766937669</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>110</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>109.2859583</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>303.109565120396</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>303.109565120396</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>110</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>18.7927593107571</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>69.76744055</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>277.874396135266</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>277.874396135266</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>132</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>40.74176943</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>183.133658477983</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>183.133658477983</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>132</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>46.395484431212</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>45.19916753</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>1682.96296296296</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>1682.96296296296</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>700</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>32.16404374</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>46.3317073217063</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>46.3317073217063</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>700</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>7.9589104323405</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>39.43923292</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>1225.07678410117</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>1225.07678410117</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="D21" s="6" t="n">
+        <v>73</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>68.1893743</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="D22" s="6" t="n">
+        <v>73</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D23" s="6" t="n">
+        <v>120</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>60.64650195</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>340.043478260869</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>340.043478260869</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D24" s="6" t="n">
+        <v>120</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>5.0796973239683</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>140.8612533</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>3484.17391304348</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>3484.17391304348</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D25" s="6" t="n">
+        <v>74</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>38.13104837</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>22.2771308148611</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>52.62885675</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="D26" s="6" t="n">
+        <v>94</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>17.18357041</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="D27" s="6" t="n">
+        <v>68</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>92.05884388</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>12.9614693862591</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>44.18219015</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>255.065217455071</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>255.065217455071</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="D28" s="6" t="n">
+        <v>68</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>15.8670241369244</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>447.2271782</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>1786.95652173913</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>1786.95652173913</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="D29" s="6" t="n">
+        <v>168</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>48.55500417</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>5.9652201118816</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>185.4257014</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>661.073170561108</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>661.073170561108</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="D30" s="6" t="n">
+        <v>73</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>81.78751095</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>18.1786971830986</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>103.0642534</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="D31" s="6" t="n">
+        <v>148</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>90.82039063</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>19.7702717332467</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>66.99777467</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D32" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>138.4426437</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>314.713043550195</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>314.713043550195</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D33" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>10.6130959436713</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>37.5761124</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D34" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>70.65449111</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>1920.24529660616</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>1920.24529660616</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D35" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D36" s="6" t="n">
+        <v>120</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>129.1017662</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D37" s="6" t="n">
+        <v>120</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>13.4542583537082</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>136.9401816</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>179</v>
+      </c>
+      <c r="D38" s="6" t="n">
+        <v>179</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>62.81986415</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>179</v>
+      </c>
+      <c r="D39" s="6" t="n">
+        <v>179</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="D40" s="6" t="n">
+        <v>113</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>92.04438506</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="D41" s="6" t="n">
+        <v>113</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D42" s="6" t="n">
+        <v>140</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>119.9515607</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>314.713043550195</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>314.713043550195</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D43" s="6" t="n">
+        <v>140</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D44" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>111.1657614</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D45" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>7.59295847115031</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>115.678228</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D46" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>56.4248001</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D47" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>13.0064207070594</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <v>22.80088017</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D48" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D49" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D50" s="6" t="n">
+        <v>120</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>139.1207513</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D51" s="6" t="n">
+        <v>120</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>9.60336494452785</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>165.7955664</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="D52" s="6" t="n">
+        <v>180</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>41.10025186</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>510.117646938796</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>510.117646938796</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="D53" s="6" t="n">
+        <v>180</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>7.1687652993939</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>86.97380591</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>224.640400250156</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>224.640400250156</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>265</v>
+      </c>
+      <c r="D54" s="6" t="n">
+        <v>265</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>10.19766882</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>5.64738272452598</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>39.36946586</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>965</v>
+      </c>
+      <c r="D55" s="6" t="n">
+        <v>965</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>9.59169388334339</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>11.90918431</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>965</v>
+      </c>
+      <c r="D56" s="6" t="n">
+        <v>965</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>17.82170147</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="D57" s="6" t="n">
+        <v>119</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>79.71774684</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="D58" s="6" t="n">
+        <v>119</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>159</v>
+      </c>
+      <c r="D59" s="6" t="n">
+        <v>159</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>61.53991313</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>159</v>
+      </c>
+      <c r="D60" s="6" t="n">
+        <v>159</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>10.480251860332</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>58.77958173</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>312</v>
+      </c>
+      <c r="D61" s="6" t="n">
+        <v>312</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>40.90035685</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>312</v>
+      </c>
+      <c r="D62" s="6" t="n">
+        <v>312</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>412</v>
+      </c>
+      <c r="D63" s="6" t="n">
+        <v>412</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>16.13711754</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>365</v>
+      </c>
+      <c r="D64" s="6" t="n">
+        <v>365</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>36.05092706</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>7.99314285714286</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <v>58.74844704</v>
+      </c>
+      <c r="I64" s="0" t="n">
+        <v>43.3505226579923</v>
+      </c>
+      <c r="J64" s="0" t="n">
+        <v>43.3505226579923</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>365</v>
+      </c>
+      <c r="D65" s="6" t="n">
+        <v>365</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>452</v>
+      </c>
+      <c r="D66" s="6" t="n">
+        <v>452</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>51.64578176</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>9.52024803643196</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <v>46.10680329</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>452</v>
+      </c>
+      <c r="D67" s="6" t="n">
+        <v>452</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G67" s="0" t="n">
+        <v>16.3138277521596</v>
+      </c>
+      <c r="H67" s="0" t="n">
+        <v>40.05351149</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="D68" s="6" t="n">
+        <v>59</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>64.57753223</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="D69" s="6" t="n">
+        <v>69</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>133.1442223</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>7.34765137670876</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <v>155.1165567</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="D70" s="6" t="n">
+        <v>69</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
plotted 2012 pump 15n and 13c in 2017 subplots
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="2017-fluxes" sheetId="1" state="visible" r:id="rId2"/>
@@ -1049,7 +1049,371 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2017 P1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fz C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.12177386572676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.32957111802758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.17726210868461</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.18437848409334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>168</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="86474731"/>
+        <c:axId val="34432666"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="86474731"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (mg/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="34432666"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="34432666"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="86474731"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1247,11 +1611,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="38423281"/>
-        <c:axId val="15765328"/>
+        <c:axId val="98243568"/>
+        <c:axId val="71985109"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="38423281"/>
+        <c:axId val="98243568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1307,12 +1671,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15765328"/>
+        <c:crossAx val="71985109"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="15765328"/>
+        <c:axId val="71985109"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1377,7 +1741,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38423281"/>
+        <c:crossAx val="98243568"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1425,7 +1789,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1611,11 +1975,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="33056632"/>
-        <c:axId val="12946567"/>
+        <c:axId val="61094318"/>
+        <c:axId val="60981215"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33056632"/>
+        <c:axId val="61094318"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,12 +2035,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12946567"/>
+        <c:crossAx val="60981215"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="12946567"/>
+        <c:axId val="60981215"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1741,7 +2105,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33056632"/>
+        <c:crossAx val="61094318"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1789,7 +2153,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1987,11 +2351,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="82839885"/>
-        <c:axId val="92066804"/>
+        <c:axId val="25833512"/>
+        <c:axId val="92818000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82839885"/>
+        <c:axId val="25833512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2047,12 +2411,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92066804"/>
+        <c:crossAx val="92818000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92066804"/>
+        <c:axId val="92818000"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2117,372 +2481,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82839885"/>
+        <c:crossAx val="25833512"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>2017 P1</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'martin power law'!$C$1:$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fz C flux organic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:marker>
-              <c:symbol val="square"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'martin power law'!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2.12177386572676</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.32957111802758</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.17726210868461</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.18437848409334</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'martin power law'!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>168</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="82639849"/>
-        <c:axId val="97472075"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="82639849"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Org C flux (mg/m2/day)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="97472075"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="97472075"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Depth (m)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="82639849"/>
-        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2544,9 +2544,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>66960</xdr:colOff>
+      <xdr:colOff>66600</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2554,8 +2554,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4845240" y="86040"/>
-        <a:ext cx="5356800" cy="4483080"/>
+        <a:off x="4847760" y="86040"/>
+        <a:ext cx="5365440" cy="4482720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2574,9 +2574,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>48600</xdr:colOff>
+      <xdr:colOff>48240</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>150840</xdr:rowOff>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2584,8 +2584,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4865760" y="5411880"/>
-        <a:ext cx="5317920" cy="4817520"/>
+        <a:off x="4868280" y="5411880"/>
+        <a:ext cx="5326560" cy="4817160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2604,9 +2604,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>765000</xdr:colOff>
+      <xdr:colOff>764640</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2614,8 +2614,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10463400" y="0"/>
-        <a:ext cx="5351400" cy="4483080"/>
+        <a:off x="10474920" y="0"/>
+        <a:ext cx="5358600" cy="4482720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2634,9 +2634,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>691920</xdr:colOff>
+      <xdr:colOff>691560</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2644,8 +2644,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10429200" y="5192280"/>
-        <a:ext cx="5312520" cy="4817520"/>
+        <a:off x="10440720" y="5192280"/>
+        <a:ext cx="5319720" cy="4817160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2665,11 +2665,11 @@
   </sheetPr>
   <dimension ref="A1:N920"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D73" activeCellId="0" sqref="D73"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
   </cols>
@@ -3593,9 +3593,7 @@
       <c r="I30" s="1" t="n">
         <v>103.0642534</v>
       </c>
-      <c r="M30" s="2" t="n">
-        <v>21.7209</v>
-      </c>
+      <c r="M30" s="2"/>
       <c r="N30" s="2" t="n">
         <v>-22.9725</v>
       </c>
@@ -3631,9 +3629,7 @@
       <c r="L31" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="M31" s="2" t="n">
-        <v>51.2103</v>
-      </c>
+      <c r="M31" s="2"/>
       <c r="N31" s="2" t="n">
         <v>-25.9195</v>
       </c>
@@ -3697,9 +3693,7 @@
       <c r="I33" s="1" t="n">
         <v>37.5761124</v>
       </c>
-      <c r="M33" s="2" t="n">
-        <v>36.8276</v>
-      </c>
+      <c r="M33" s="2"/>
       <c r="N33" s="2" t="n">
         <v>-26.0099</v>
       </c>
@@ -3810,9 +3804,7 @@
       <c r="I37" s="1" t="n">
         <v>136.9401816</v>
       </c>
-      <c r="M37" s="2" t="n">
-        <v>37.3267</v>
-      </c>
+      <c r="M37" s="2"/>
       <c r="N37" s="2" t="n">
         <v>-23.3694</v>
       </c>
@@ -4026,9 +4018,7 @@
       <c r="I45" s="1" t="n">
         <v>115.678228</v>
       </c>
-      <c r="M45" s="2" t="n">
-        <v>19.4703</v>
-      </c>
+      <c r="M45" s="2"/>
       <c r="N45" s="2" t="n">
         <v>-24.284</v>
       </c>
@@ -4059,7 +4049,7 @@
         <v>30</v>
       </c>
       <c r="M46" s="2" t="n">
-        <v>35.27</v>
+        <v>8.936</v>
       </c>
       <c r="N46" s="2" t="n">
         <v>-26.7068</v>
@@ -4090,9 +4080,7 @@
       <c r="I47" s="1" t="n">
         <v>22.80088017</v>
       </c>
-      <c r="M47" s="2" t="n">
-        <v>39.2771</v>
-      </c>
+      <c r="M47" s="2"/>
       <c r="N47" s="2" t="n">
         <v>-22.4823</v>
       </c>
@@ -4197,9 +4185,7 @@
       <c r="I51" s="1" t="n">
         <v>165.7955664</v>
       </c>
-      <c r="M51" s="2" t="n">
-        <v>32.0272</v>
-      </c>
+      <c r="M51" s="2"/>
       <c r="N51" s="2" t="n">
         <v>-22.8841</v>
       </c>
@@ -4266,9 +4252,7 @@
       <c r="K53" s="1" t="n">
         <v>224.640400250156</v>
       </c>
-      <c r="M53" s="2" t="n">
-        <v>17.2123</v>
-      </c>
+      <c r="M53" s="2"/>
       <c r="N53" s="2" t="n">
         <v>-23.7632</v>
       </c>
@@ -4302,7 +4286,7 @@
         <v>39.36946586</v>
       </c>
       <c r="M54" s="2" t="n">
-        <v>11.4427</v>
+        <v>8.0633</v>
       </c>
       <c r="N54" s="2" t="n">
         <v>-17.581</v>
@@ -4466,9 +4450,7 @@
       <c r="I60" s="1" t="n">
         <v>58.77958173</v>
       </c>
-      <c r="M60" s="2" t="n">
-        <v>22.9036</v>
-      </c>
+      <c r="M60" s="2"/>
       <c r="N60" s="2" t="n">
         <v>-24.5682</v>
       </c>
@@ -4605,7 +4587,7 @@
       <c r="F65" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M65" s="1"/>
+      <c r="M65" s="2"/>
       <c r="N65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4636,9 +4618,7 @@
       <c r="I66" s="1" t="n">
         <v>46.10680329</v>
       </c>
-      <c r="M66" s="2" t="n">
-        <v>40.73</v>
-      </c>
+      <c r="M66" s="2"/>
       <c r="N66" s="2" t="n">
         <v>-20.751</v>
       </c>
@@ -4668,9 +4648,7 @@
       <c r="I67" s="1" t="n">
         <v>40.05351149</v>
       </c>
-      <c r="M67" s="2" t="n">
-        <v>40.5119</v>
-      </c>
+      <c r="M67" s="2"/>
       <c r="N67" s="2" t="n">
         <v>-28.2913</v>
       </c>
@@ -4728,9 +4706,7 @@
       <c r="I69" s="1" t="n">
         <v>155.1165567</v>
       </c>
-      <c r="M69" s="2" t="n">
-        <v>17.4358</v>
-      </c>
+      <c r="M69" s="2"/>
       <c r="N69" s="2" t="n">
         <v>-20.6818</v>
       </c>
@@ -8175,11 +8151,11 @@
   </sheetPr>
   <dimension ref="A1:C954"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B103" activeCellId="0" sqref="B103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.11"/>
   </cols>
@@ -13268,8 +13244,8 @@
   </sheetPr>
   <dimension ref="A1:BJ70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW5" activeCellId="0" sqref="AW5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24614,11 +24590,11 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U57" activeCellId="0" sqref="U57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.29"/>

</xml_diff>

<commit_message>
figured out n2 rate prod xlsx for 2018
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2017-fluxes" sheetId="1" state="visible" r:id="rId2"/>
@@ -1054,7 +1054,1820 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2017 P1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fz C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.12177386572676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.32957111802758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.17726210868461</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.18437848409334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>168</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="20420340"/>
+        <c:axId val="28613461"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="20420340"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (mg/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="28613461"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="28613461"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="20420340"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2017 P2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$8:$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fz C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$9:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.78334661696259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.03416289552556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.32232450014019</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.828830860507312</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.47769543896914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.96315848404831</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$B$9:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>452</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="93804552"/>
+        <c:axId val="78192550"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="93804552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (mg C/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="78192550"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="78192550"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="93804552"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2017 P1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fz C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.22176805440372</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.32957111802758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.69507659059645</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.01848578146802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.12177386572676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.32957111802758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.17726210868461</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.18437848409334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="66054043"/>
+        <c:axId val="44749672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="66054043"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (mg/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="44749672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="44749672"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="66054043"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2017 P2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$8:$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fz C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$D$9:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.92270191494882</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.03416289552556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.12405628133949</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.38428996320923</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.1708144776278</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.595090805172</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$9:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.78334661696259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.03416289552556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.32232450014019</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.828830860507312</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.47769543896914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.96315848404831</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="46553969"/>
+        <c:axId val="68489463"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="46553969"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (mg C/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="68489463"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="68489463"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="46553969"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'protein power function P1'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normalized to F100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="579d1c"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'protein power function P1'!$D$2:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>329.466918726015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>255.065217455071</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1786.95652173913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>240.000000011294</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>952.869565217391</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>303.109565120396</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>277.874396135266</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>340.043478260869</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3484.17391304348</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>183.133658477983</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1682.96296296296</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1380.74796747967</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>661.073170561108</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>601.724877856229</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1286.93766937669</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>46.3317073217063</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'protein power function P1'!$C$2:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="37420940"/>
+        <c:axId val="53579098"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="37420940"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="53579098"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="53579098"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37420940"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1359,11 +3172,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="85185264"/>
-        <c:axId val="51332119"/>
+        <c:axId val="55336482"/>
+        <c:axId val="53894874"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85185264"/>
+        <c:axId val="55336482"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1391,12 +3204,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51332119"/>
+        <c:crossAx val="53894874"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51332119"/>
+        <c:axId val="53894874"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1433,1820 +3246,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85185264"/>
-        <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>2017 P1</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'martin power law'!$C$1:$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fz C flux organic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:marker>
-              <c:symbol val="square"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'martin power law'!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2.12177386572676</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.32957111802758</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.17726210868461</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.18437848409334</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'martin power law'!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>168</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="21335721"/>
-        <c:axId val="16787599"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="21335721"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Org C flux (mg/m2/day)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="16787599"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="16787599"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Depth (m)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="21335721"/>
-        <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>2017 P2</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'martin power law'!$C$8:$C$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fz C flux organic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="square"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'martin power law'!$C$9:$C$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>6.78334661696259</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.03416289552556</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.32232450014019</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.828830860507312</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.47769543896914</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.96315848404831</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'martin power law'!$B$9:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>265</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>365</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>452</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="28577376"/>
-        <c:axId val="43516074"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="28577376"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Org C flux (mg C/m2/day)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="43516074"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="43516074"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Depth (m)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="28577376"/>
-        <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>2017 P1</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'martin power law'!$C$1:$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fz C flux organic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:marker>
-              <c:symbol val="square"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'martin power law'!$D$2:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.22176805440372</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.32957111802758</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.69507659059645</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.01848578146802</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'martin power law'!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2.12177386572676</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.32957111802758</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.17726210868461</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.18437848409334</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="92901544"/>
-        <c:axId val="61801520"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="92901544"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Org C flux (mg/m2/day)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="61801520"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="61801520"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Depth (m)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="92901544"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>2017 P2</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'martin power law'!$C$8:$C$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fz C flux organic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="square"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'martin power law'!$D$9:$D$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.92270191494882</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.03416289552556</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.12405628133949</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.38428996320923</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.1708144776278</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12.595090805172</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'martin power law'!$C$9:$C$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>6.78334661696259</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.03416289552556</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.32232450014019</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.828830860507312</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.47769543896914</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.96315848404831</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="76561748"/>
-        <c:axId val="15071324"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="76561748"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Org C flux (mg C/m2/day)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="15071324"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="15071324"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Depth (m)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="76561748"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'protein power function P1'!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Normalized to F100</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="579d1c"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="579d1c"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'protein power function P1'!$D$2:$D$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>329.466918726015</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>255.065217455071</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1786.95652173913</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>240.000000011294</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>952.869565217391</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>303.109565120396</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>277.874396135266</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>340.043478260869</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3484.17391304348</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>183.133658477983</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1682.96296296296</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1380.74796747967</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>661.073170561108</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>601.724877856229</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1286.93766937669</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>46.3317073217063</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'protein power function P1'!$C$2:$C$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>168</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>355</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>355</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>700</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="64938373"/>
-        <c:axId val="13499317"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="64938373"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="13499317"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="13499317"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="64938373"/>
+        <c:crossAx val="55336482"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25617,7 +25617,7 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -26137,7 +26137,7 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fit all rate profiles to normalized power laws in xlsx
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -1060,7 +1060,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart117.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart139.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1246,11 +1246,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="74904987"/>
-        <c:axId val="77019745"/>
+        <c:axId val="7114776"/>
+        <c:axId val="17158992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74904987"/>
+        <c:axId val="7114776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,12 +1306,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77019745"/>
+        <c:crossAx val="17158992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77019745"/>
+        <c:axId val="17158992"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1376,7 +1376,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74904987"/>
+        <c:crossAx val="7114776"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1424,7 +1424,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart118.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart140.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1622,11 +1622,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="50273238"/>
-        <c:axId val="53075414"/>
+        <c:axId val="52156180"/>
+        <c:axId val="21892608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50273238"/>
+        <c:axId val="52156180"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1682,12 +1682,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53075414"/>
+        <c:crossAx val="21892608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53075414"/>
+        <c:axId val="21892608"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1752,7 +1752,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50273238"/>
+        <c:crossAx val="52156180"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1800,7 +1800,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart119.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart141.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1986,11 +1986,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="57425988"/>
-        <c:axId val="75988915"/>
+        <c:axId val="75132275"/>
+        <c:axId val="54736723"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57425988"/>
+        <c:axId val="75132275"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2046,12 +2046,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75988915"/>
+        <c:crossAx val="54736723"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75988915"/>
+        <c:axId val="54736723"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2116,7 +2116,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57425988"/>
+        <c:crossAx val="75132275"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2164,7 +2164,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart120.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart142.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2362,11 +2362,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="45055964"/>
-        <c:axId val="4446924"/>
+        <c:axId val="79748563"/>
+        <c:axId val="33068540"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45055964"/>
+        <c:axId val="79748563"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2422,12 +2422,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4446924"/>
+        <c:crossAx val="33068540"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4446924"/>
+        <c:axId val="33068540"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2492,7 +2492,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45055964"/>
+        <c:crossAx val="79748563"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2540,7 +2540,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart121.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart143.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2773,11 +2773,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="51479159"/>
-        <c:axId val="21592867"/>
+        <c:axId val="17600630"/>
+        <c:axId val="85993977"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51479159"/>
+        <c:axId val="17600630"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2805,12 +2805,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21592867"/>
+        <c:crossAx val="85993977"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21592867"/>
+        <c:axId val="85993977"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2847,7 +2847,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51479159"/>
+        <c:crossAx val="17600630"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2874,7 +2874,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart122.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart144.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3182,11 +3182,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="42858692"/>
-        <c:axId val="17429128"/>
+        <c:axId val="31680549"/>
+        <c:axId val="10806179"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42858692"/>
+        <c:axId val="31680549"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3214,12 +3214,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17429128"/>
+        <c:crossAx val="10806179"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17429128"/>
+        <c:axId val="10806179"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3256,7 +3256,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42858692"/>
+        <c:crossAx val="31680549"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3489,8 +3489,8 @@
   </sheetPr>
   <dimension ref="A1:P920"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P35" activeCellId="0" sqref="P35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
added in the new ctl bottle and 2017 p1 rates to the flux 2017 and 2018
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -1063,7 +1063,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart73.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1249,11 +1249,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="88139170"/>
-        <c:axId val="79311993"/>
+        <c:axId val="3845834"/>
+        <c:axId val="23508736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88139170"/>
+        <c:axId val="3845834"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,12 +1309,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79311993"/>
+        <c:crossAx val="23508736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79311993"/>
+        <c:axId val="23508736"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1379,7 +1379,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88139170"/>
+        <c:crossAx val="3845834"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1427,7 +1427,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart74.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1625,11 +1625,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="9860334"/>
-        <c:axId val="47331823"/>
+        <c:axId val="56434906"/>
+        <c:axId val="32462307"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9860334"/>
+        <c:axId val="56434906"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,12 +1685,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47331823"/>
+        <c:crossAx val="32462307"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47331823"/>
+        <c:axId val="32462307"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1755,7 +1755,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9860334"/>
+        <c:crossAx val="56434906"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1803,7 +1803,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart75.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1989,11 +1989,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="20886806"/>
-        <c:axId val="21702336"/>
+        <c:axId val="28800667"/>
+        <c:axId val="5777090"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20886806"/>
+        <c:axId val="28800667"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2049,12 +2049,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21702336"/>
+        <c:crossAx val="5777090"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21702336"/>
+        <c:axId val="5777090"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2119,7 +2119,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20886806"/>
+        <c:crossAx val="28800667"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2167,7 +2167,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart76.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2365,11 +2365,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="32486102"/>
-        <c:axId val="79979301"/>
+        <c:axId val="18406711"/>
+        <c:axId val="29610330"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="32486102"/>
+        <c:axId val="18406711"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2425,12 +2425,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79979301"/>
+        <c:crossAx val="29610330"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79979301"/>
+        <c:axId val="29610330"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2495,7 +2495,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32486102"/>
+        <c:crossAx val="18406711"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2543,7 +2543,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart77.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2776,11 +2776,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="26516544"/>
-        <c:axId val="16685732"/>
+        <c:axId val="63424294"/>
+        <c:axId val="26065057"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="26516544"/>
+        <c:axId val="63424294"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2808,12 +2808,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16685732"/>
+        <c:crossAx val="26065057"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="16685732"/>
+        <c:axId val="26065057"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2850,7 +2850,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26516544"/>
+        <c:crossAx val="63424294"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2877,7 +2877,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart78.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3185,11 +3185,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="82365111"/>
-        <c:axId val="90983656"/>
+        <c:axId val="54503105"/>
+        <c:axId val="88960353"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82365111"/>
+        <c:axId val="54503105"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3217,12 +3217,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90983656"/>
+        <c:crossAx val="88960353"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90983656"/>
+        <c:axId val="88960353"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3259,7 +3259,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82365111"/>
+        <c:crossAx val="54503105"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3492,8 +3492,8 @@
   </sheetPr>
   <dimension ref="A1:Q920"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L46" activeCellId="0" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3610,6 +3610,15 @@
       <c r="K3" s="1" t="n">
         <v>329.466918726015</v>
       </c>
+      <c r="L3" s="0" t="n">
+        <v>13.75</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>2.12205443079987</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>7.25</v>
+      </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
@@ -3724,6 +3733,12 @@
       </c>
       <c r="K7" s="1" t="n">
         <v>240.000000011294</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>8.17955525900485</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -3787,6 +3802,12 @@
       <c r="G9" s="1" t="n">
         <v>132.0557482</v>
       </c>
+      <c r="L9" s="0" t="n">
+        <v>17.25</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>5.32442748060598</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
@@ -3840,6 +3861,15 @@
       <c r="G11" s="1" t="n">
         <v>103.7328318</v>
       </c>
+      <c r="L11" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>4.11549950111472</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>1.25</v>
+      </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
@@ -3899,6 +3929,15 @@
       <c r="K13" s="1" t="n">
         <v>601.724877856229</v>
       </c>
+      <c r="L13" s="0" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>3.39891185055482</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
@@ -3964,6 +4003,12 @@
       <c r="K15" s="1" t="n">
         <v>303.109565120396</v>
       </c>
+      <c r="L15" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>5.83029096227096</v>
+      </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
@@ -4029,6 +4074,15 @@
       <c r="K17" s="1" t="n">
         <v>183.133658477983</v>
       </c>
+      <c r="L17" s="0" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>2.11630360602566</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>11.5</v>
+      </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
@@ -4468,12 +4522,6 @@
       <c r="I31" s="1" t="n">
         <v>66.99777467</v>
       </c>
-      <c r="L31" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="M31" s="0" t="n">
-        <v>1.51114571520455</v>
-      </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2" t="n">
         <v>-25.9195</v>
@@ -4508,10 +4556,13 @@
         <v>314.713043550195</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M32" s="0" t="n">
-        <v>2.52542014905108</v>
+        <v>7.92246387321939</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -4577,6 +4628,15 @@
       <c r="K34" s="1" t="n">
         <v>1920.24529660616</v>
       </c>
+      <c r="L34" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="M34" s="0" t="n">
+        <v>2.01486095360607</v>
+      </c>
+      <c r="N34" s="0" t="n">
+        <v>3.5</v>
+      </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="0" t="n">
@@ -4628,10 +4688,13 @@
         <v>129.1017662</v>
       </c>
       <c r="L36" s="0" t="n">
-        <v>16</v>
+        <v>18.5</v>
       </c>
       <c r="M36" s="0" t="n">
-        <v>2.69378149232115</v>
+        <v>3.11468485049633</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <v>12.25</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -4689,10 +4752,13 @@
         <v>62.81986415</v>
       </c>
       <c r="L38" s="0" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M38" s="0" t="n">
-        <v>1.95189654880588</v>
+        <v>2.14078976320645</v>
+      </c>
+      <c r="N38" s="0" t="n">
+        <v>5.5</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -4742,10 +4808,13 @@
         <v>92.04438506</v>
       </c>
       <c r="L40" s="0" t="n">
-        <v>34</v>
+        <v>36.75</v>
       </c>
       <c r="M40" s="0" t="n">
-        <v>4.80415754312583</v>
+        <v>5.19272910911395</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <v>20</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -4806,6 +4875,9 @@
       <c r="M42" s="0" t="n">
         <v>0.78705506000237</v>
       </c>
+      <c r="N42" s="0" t="n">
+        <v>5.25</v>
+      </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
@@ -4854,10 +4926,13 @@
         <v>111.1657614</v>
       </c>
       <c r="L44" s="0" t="n">
-        <v>29</v>
+        <v>31.75</v>
       </c>
       <c r="M44" s="0" t="n">
-        <v>4.88247895483209</v>
+        <v>5.34547264882479</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <v>3.25</v>
       </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -4915,10 +4990,13 @@
         <v>56.4248001</v>
       </c>
       <c r="L46" s="0" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M46" s="0" t="n">
-        <v>1.88893214400569</v>
+        <v>1.63707452480493</v>
+      </c>
+      <c r="N46" s="0" t="n">
+        <v>3.5</v>
       </c>
       <c r="O46" s="2" t="n">
         <v>8.936</v>
@@ -4998,12 +5076,6 @@
       <c r="F49" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L49" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="M49" s="0" t="n">
-        <v>3.53558820867151</v>
-      </c>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
     </row>
@@ -5029,6 +5101,15 @@
       <c r="G50" s="1" t="n">
         <v>139.1207513</v>
       </c>
+      <c r="L50" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="M50" s="0" t="n">
+        <v>3.87231089521166</v>
+      </c>
+      <c r="N50" s="0" t="n">
+        <v>5.25</v>
+      </c>
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
     </row>
@@ -5091,10 +5172,13 @@
         <v>510.117646938796</v>
       </c>
       <c r="L52" s="0" t="n">
-        <v>39</v>
+        <v>41.75</v>
       </c>
       <c r="M52" s="0" t="n">
-        <v>2.45561178720739</v>
+        <v>2.62876390040791</v>
+      </c>
+      <c r="N52" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>

</xml_diff>

<commit_message>
scraped nuts data for 2018 and 2017 and plotted in rate flux mega plots
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -1063,7 +1063,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart134.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1249,11 +1249,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="3845834"/>
-        <c:axId val="23508736"/>
+        <c:axId val="55174777"/>
+        <c:axId val="73934877"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3845834"/>
+        <c:axId val="55174777"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,12 +1309,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23508736"/>
+        <c:crossAx val="73934877"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="23508736"/>
+        <c:axId val="73934877"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1379,7 +1379,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3845834"/>
+        <c:crossAx val="55174777"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1427,7 +1427,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart135.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1625,11 +1625,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="56434906"/>
-        <c:axId val="32462307"/>
+        <c:axId val="14297363"/>
+        <c:axId val="57528579"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56434906"/>
+        <c:axId val="14297363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,12 +1685,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32462307"/>
+        <c:crossAx val="57528579"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32462307"/>
+        <c:axId val="57528579"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1755,7 +1755,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56434906"/>
+        <c:crossAx val="14297363"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1803,7 +1803,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart136.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1989,11 +1989,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="28800667"/>
-        <c:axId val="5777090"/>
+        <c:axId val="82128240"/>
+        <c:axId val="82197627"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="28800667"/>
+        <c:axId val="82128240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2049,12 +2049,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5777090"/>
+        <c:crossAx val="82197627"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5777090"/>
+        <c:axId val="82197627"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2119,7 +2119,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28800667"/>
+        <c:crossAx val="82128240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2167,7 +2167,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart137.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2365,11 +2365,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="18406711"/>
-        <c:axId val="29610330"/>
+        <c:axId val="10579126"/>
+        <c:axId val="65788191"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="18406711"/>
+        <c:axId val="10579126"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2425,12 +2425,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29610330"/>
+        <c:crossAx val="65788191"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29610330"/>
+        <c:axId val="65788191"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2495,7 +2495,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18406711"/>
+        <c:crossAx val="10579126"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2543,7 +2543,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart138.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2776,11 +2776,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="63424294"/>
-        <c:axId val="26065057"/>
+        <c:axId val="49722379"/>
+        <c:axId val="47858843"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63424294"/>
+        <c:axId val="49722379"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2808,12 +2808,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26065057"/>
+        <c:crossAx val="47858843"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="26065057"/>
+        <c:axId val="47858843"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2850,7 +2850,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63424294"/>
+        <c:crossAx val="49722379"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2877,7 +2877,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart139.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3185,11 +3185,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="54503105"/>
-        <c:axId val="88960353"/>
+        <c:axId val="97591312"/>
+        <c:axId val="97118852"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54503105"/>
+        <c:axId val="97591312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3217,12 +3217,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88960353"/>
+        <c:crossAx val="97118852"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88960353"/>
+        <c:axId val="97118852"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3259,7 +3259,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54503105"/>
+        <c:crossAx val="97591312"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3301,9 +3301,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>64800</xdr:colOff>
+      <xdr:colOff>64440</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3311,8 +3311,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4859280" y="86040"/>
-        <a:ext cx="5403600" cy="4480920"/>
+        <a:off x="4861800" y="86040"/>
+        <a:ext cx="5411880" cy="4480560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3331,9 +3331,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>46440</xdr:colOff>
+      <xdr:colOff>46080</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>148680</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3341,8 +3341,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4879800" y="5411880"/>
-        <a:ext cx="5364720" cy="4815360"/>
+        <a:off x="4882320" y="5411880"/>
+        <a:ext cx="5373000" cy="4815000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3361,9 +3361,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>762840</xdr:colOff>
+      <xdr:colOff>762480</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3371,8 +3371,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10526400" y="0"/>
-        <a:ext cx="5391000" cy="4480920"/>
+        <a:off x="10537560" y="0"/>
+        <a:ext cx="5398560" cy="4480560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3391,9 +3391,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>689760</xdr:colOff>
+      <xdr:colOff>689400</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3401,8 +3401,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10492200" y="5192280"/>
-        <a:ext cx="5352120" cy="4815360"/>
+        <a:off x="10503360" y="5192280"/>
+        <a:ext cx="5359680" cy="4815000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3426,9 +3426,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>504000</xdr:colOff>
+      <xdr:colOff>503640</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
+      <xdr:rowOff>65520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3436,8 +3436,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5621040" y="210240"/>
-        <a:ext cx="4697280" cy="4407120"/>
+        <a:off x="5628600" y="210240"/>
+        <a:ext cx="4704840" cy="4406760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3461,9 +3461,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>761760</xdr:colOff>
+      <xdr:colOff>761400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>122760</xdr:rowOff>
+      <xdr:rowOff>122400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3471,8 +3471,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5601240" y="458640"/>
-        <a:ext cx="5792760" cy="3240360"/>
+        <a:off x="5608800" y="458640"/>
+        <a:ext cx="5801400" cy="3240000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3492,11 +3492,11 @@
   </sheetPr>
   <dimension ref="A1:Q920"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L46" activeCellId="0" sqref="L46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
   </cols>
@@ -9117,7 +9117,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.11"/>
   </cols>
@@ -25556,7 +25556,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.29"/>
@@ -25769,7 +25769,7 @@
       <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -26289,7 +26289,7 @@
       <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
plotted 2017 protein and cn of flux
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -967,7 +967,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1063,7 +1063,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart134.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart87.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1249,11 +1249,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="55174777"/>
-        <c:axId val="73934877"/>
+        <c:axId val="49318673"/>
+        <c:axId val="86099962"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55174777"/>
+        <c:axId val="49318673"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,12 +1309,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73934877"/>
+        <c:crossAx val="86099962"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73934877"/>
+        <c:axId val="86099962"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1379,7 +1379,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55174777"/>
+        <c:crossAx val="49318673"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1427,7 +1427,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart135.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart88.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1625,11 +1625,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="14297363"/>
-        <c:axId val="57528579"/>
+        <c:axId val="28099833"/>
+        <c:axId val="48082877"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="14297363"/>
+        <c:axId val="28099833"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,12 +1685,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57528579"/>
+        <c:crossAx val="48082877"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57528579"/>
+        <c:axId val="48082877"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1755,7 +1755,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14297363"/>
+        <c:crossAx val="28099833"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1803,7 +1803,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart136.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart89.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1989,11 +1989,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="82128240"/>
-        <c:axId val="82197627"/>
+        <c:axId val="30403148"/>
+        <c:axId val="29242847"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82128240"/>
+        <c:axId val="30403148"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2049,12 +2049,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82197627"/>
+        <c:crossAx val="29242847"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82197627"/>
+        <c:axId val="29242847"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2119,7 +2119,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82128240"/>
+        <c:crossAx val="30403148"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2167,7 +2167,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart137.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart90.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2365,11 +2365,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="10579126"/>
-        <c:axId val="65788191"/>
+        <c:axId val="99514331"/>
+        <c:axId val="85036926"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="10579126"/>
+        <c:axId val="99514331"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2425,12 +2425,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65788191"/>
+        <c:crossAx val="85036926"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65788191"/>
+        <c:axId val="85036926"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2495,7 +2495,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10579126"/>
+        <c:crossAx val="99514331"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2543,7 +2543,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart138.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart91.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2776,11 +2776,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="49722379"/>
-        <c:axId val="47858843"/>
+        <c:axId val="25628793"/>
+        <c:axId val="51226124"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49722379"/>
+        <c:axId val="25628793"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2808,12 +2808,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47858843"/>
+        <c:crossAx val="51226124"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47858843"/>
+        <c:axId val="51226124"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2850,7 +2850,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49722379"/>
+        <c:crossAx val="25628793"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2877,7 +2877,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart139.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart92.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3185,11 +3185,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="97591312"/>
-        <c:axId val="97118852"/>
+        <c:axId val="45919150"/>
+        <c:axId val="52012145"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97591312"/>
+        <c:axId val="45919150"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3217,12 +3217,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97118852"/>
+        <c:crossAx val="52012145"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97118852"/>
+        <c:axId val="52012145"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3259,7 +3259,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97591312"/>
+        <c:crossAx val="45919150"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3301,9 +3301,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>64440</xdr:colOff>
+      <xdr:colOff>64080</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3311,8 +3311,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4861800" y="86040"/>
-        <a:ext cx="5411880" cy="4480560"/>
+        <a:off x="4864320" y="86040"/>
+        <a:ext cx="5420520" cy="4480200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3331,9 +3331,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>46080</xdr:colOff>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>148320</xdr:rowOff>
+      <xdr:rowOff>147960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3341,8 +3341,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4882320" y="5411880"/>
-        <a:ext cx="5373000" cy="4815000"/>
+        <a:off x="4884840" y="5411880"/>
+        <a:ext cx="5381640" cy="4814640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3361,9 +3361,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>762480</xdr:colOff>
+      <xdr:colOff>762120</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3371,8 +3371,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10537560" y="0"/>
-        <a:ext cx="5398560" cy="4480560"/>
+        <a:off x="10549080" y="0"/>
+        <a:ext cx="5405760" cy="4480200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3391,9 +3391,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>689400</xdr:colOff>
+      <xdr:colOff>689040</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3401,8 +3401,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10503360" y="5192280"/>
-        <a:ext cx="5359680" cy="4815000"/>
+        <a:off x="10514880" y="5192280"/>
+        <a:ext cx="5366880" cy="4814640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3426,9 +3426,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>503640</xdr:colOff>
+      <xdr:colOff>503280</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:rowOff>65160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3436,8 +3436,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5628600" y="210240"/>
-        <a:ext cx="4704840" cy="4406760"/>
+        <a:off x="5636160" y="210240"/>
+        <a:ext cx="4712040" cy="4406400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3461,9 +3461,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>761400</xdr:colOff>
+      <xdr:colOff>761040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3471,8 +3471,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5608800" y="458640"/>
-        <a:ext cx="5801400" cy="3240000"/>
+        <a:off x="5616360" y="458640"/>
+        <a:ext cx="5810040" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3490,15 +3490,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q920"/>
+  <dimension ref="A1:Q70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="11.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3550,7 +3551,7 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3576,9 +3577,7 @@
       <c r="G2" s="1" t="n">
         <v>88.65132562</v>
       </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2" s="1" t="n">
         <v>45.2</v>
       </c>
     </row>
@@ -3610,17 +3609,15 @@
       <c r="K3" s="1" t="n">
         <v>329.466918726015</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="1" t="n">
         <v>13.75</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>2.12205443079987</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>7.25</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -3641,8 +3638,6 @@
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -3678,8 +3673,6 @@
       <c r="K5" s="1" t="n">
         <v>1380.74796747967</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -3703,8 +3696,6 @@
       <c r="H6" s="1" t="n">
         <v>6.33046700778707</v>
       </c>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -3734,15 +3725,13 @@
       <c r="K7" s="1" t="n">
         <v>240.000000011294</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7" s="1" t="n">
         <v>26.5</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="1" t="n">
         <v>8.17955525900485</v>
       </c>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="0" t="n">
+      <c r="Q7" s="1" t="n">
         <v>42.8</v>
       </c>
     </row>
@@ -3765,9 +3754,6 @@
       <c r="F8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="1" t="n">
-        <v>25.7141237285309</v>
-      </c>
       <c r="I8" s="1" t="n">
         <v>45.62906039</v>
       </c>
@@ -3777,8 +3763,6 @@
       <c r="K8" s="1" t="n">
         <v>952.869565217391</v>
       </c>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -3802,14 +3786,12 @@
       <c r="G9" s="1" t="n">
         <v>132.0557482</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9" s="1" t="n">
         <v>17.25</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9" s="1" t="n">
         <v>5.32442748060598</v>
       </c>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -3830,14 +3812,9 @@
       <c r="F10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="1" t="n">
-        <v>37.4768756857119</v>
-      </c>
       <c r="I10" s="1" t="n">
         <v>82.12926293</v>
       </c>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -3861,17 +3838,15 @@
       <c r="G11" s="1" t="n">
         <v>103.7328318</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="1" t="n">
         <v>4.11549950111472</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="1" t="n">
         <v>1.25</v>
       </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -3892,14 +3867,9 @@
       <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="1" t="n">
-        <v>18.2032700523594</v>
-      </c>
       <c r="I12" s="1" t="n">
         <v>55.80971782</v>
       </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -3929,17 +3899,15 @@
       <c r="K13" s="1" t="n">
         <v>601.724877856229</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="1" t="n">
         <v>26.5</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M13" s="1" t="n">
         <v>3.39891185055482</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N13" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -3972,8 +3940,6 @@
       <c r="K14" s="1" t="n">
         <v>1286.93766937669</v>
       </c>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -4003,14 +3969,12 @@
       <c r="K15" s="1" t="n">
         <v>303.109565120396</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="1" t="n">
         <v>5.83029096227096</v>
       </c>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -4031,9 +3995,6 @@
       <c r="F16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="1" t="n">
-        <v>18.7927593107571</v>
-      </c>
       <c r="I16" s="1" t="n">
         <v>69.76744055</v>
       </c>
@@ -4043,8 +4004,6 @@
       <c r="K16" s="1" t="n">
         <v>277.874396135266</v>
       </c>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -4074,17 +4033,15 @@
       <c r="K17" s="1" t="n">
         <v>183.133658477983</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="L17" s="1" t="n">
         <v>16.5</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="M17" s="1" t="n">
         <v>2.11630360602566</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="N17" s="1" t="n">
         <v>11.5</v>
       </c>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -4105,9 +4062,6 @@
       <c r="F18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="1" t="n">
-        <v>46.395484431212</v>
-      </c>
       <c r="I18" s="1" t="n">
         <v>45.19916753</v>
       </c>
@@ -4117,8 +4071,6 @@
       <c r="K18" s="1" t="n">
         <v>1682.96296296296</v>
       </c>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -4148,8 +4100,6 @@
       <c r="K19" s="1" t="n">
         <v>46.3317073217063</v>
       </c>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -4182,8 +4132,6 @@
       <c r="K20" s="1" t="n">
         <v>1225.07678410117</v>
       </c>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -4207,8 +4155,6 @@
       <c r="G21" s="1" t="n">
         <v>68.1893743</v>
       </c>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -4229,8 +4175,6 @@
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -4260,8 +4204,6 @@
       <c r="K23" s="1" t="n">
         <v>340.043478260869</v>
       </c>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -4294,8 +4236,6 @@
       <c r="K24" s="1" t="n">
         <v>3484.17391304348</v>
       </c>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
@@ -4319,14 +4259,9 @@
       <c r="G25" s="1" t="n">
         <v>38.13104837</v>
       </c>
-      <c r="H25" s="1" t="n">
-        <v>22.2771308148611</v>
-      </c>
       <c r="I25" s="1" t="n">
         <v>52.62885675</v>
       </c>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -4350,8 +4285,6 @@
       <c r="G26" s="1" t="n">
         <v>17.18357041</v>
       </c>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
@@ -4375,9 +4308,6 @@
       <c r="G27" s="1" t="n">
         <v>92.05884388</v>
       </c>
-      <c r="H27" s="1" t="n">
-        <v>12.9614693862591</v>
-      </c>
       <c r="I27" s="1" t="n">
         <v>44.18219015</v>
       </c>
@@ -4387,8 +4317,6 @@
       <c r="K27" s="1" t="n">
         <v>255.065217455071</v>
       </c>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
@@ -4409,9 +4337,6 @@
       <c r="F28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H28" s="1" t="n">
-        <v>15.8670241369244</v>
-      </c>
       <c r="I28" s="1" t="n">
         <v>447.2271782</v>
       </c>
@@ -4421,8 +4346,6 @@
       <c r="K28" s="1" t="n">
         <v>1786.95652173913</v>
       </c>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -4458,8 +4381,6 @@
       <c r="K29" s="1" t="n">
         <v>661.073170561108</v>
       </c>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
@@ -4483,9 +4404,6 @@
       <c r="G30" s="1" t="n">
         <v>81.78751095</v>
       </c>
-      <c r="H30" s="1" t="n">
-        <v>18.1786971830986</v>
-      </c>
       <c r="I30" s="1" t="n">
         <v>103.0642534</v>
       </c>
@@ -4516,9 +4434,6 @@
       <c r="G31" s="1" t="n">
         <v>90.82039063</v>
       </c>
-      <c r="H31" s="1" t="n">
-        <v>19.7702717332467</v>
-      </c>
       <c r="I31" s="1" t="n">
         <v>66.99777467</v>
       </c>
@@ -4555,18 +4470,16 @@
       <c r="K32" s="1" t="n">
         <v>314.713043550195</v>
       </c>
-      <c r="L32" s="0" t="n">
+      <c r="L32" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="M32" s="0" t="n">
+      <c r="M32" s="1" t="n">
         <v>7.92246387321939</v>
       </c>
-      <c r="N32" s="0" t="n">
+      <c r="N32" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="0" t="n">
+      <c r="Q32" s="1" t="n">
         <v>9.4</v>
       </c>
     </row>
@@ -4628,18 +4541,16 @@
       <c r="K34" s="1" t="n">
         <v>1920.24529660616</v>
       </c>
-      <c r="L34" s="0" t="n">
+      <c r="L34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="M34" s="0" t="n">
+      <c r="M34" s="1" t="n">
         <v>2.01486095360607</v>
       </c>
-      <c r="N34" s="0" t="n">
+      <c r="N34" s="1" t="n">
         <v>3.5</v>
       </c>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="0" t="n">
+      <c r="Q34" s="1" t="n">
         <v>21.1</v>
       </c>
     </row>
@@ -4662,8 +4573,6 @@
       <c r="F35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
@@ -4687,17 +4596,15 @@
       <c r="G36" s="1" t="n">
         <v>129.1017662</v>
       </c>
-      <c r="L36" s="0" t="n">
+      <c r="L36" s="1" t="n">
         <v>18.5</v>
       </c>
-      <c r="M36" s="0" t="n">
+      <c r="M36" s="1" t="n">
         <v>3.11468485049633</v>
       </c>
-      <c r="N36" s="0" t="n">
+      <c r="N36" s="1" t="n">
         <v>12.25</v>
       </c>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
@@ -4751,17 +4658,15 @@
       <c r="G38" s="1" t="n">
         <v>62.81986415</v>
       </c>
-      <c r="L38" s="0" t="n">
+      <c r="L38" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="M38" s="0" t="n">
+      <c r="M38" s="1" t="n">
         <v>2.14078976320645</v>
       </c>
-      <c r="N38" s="0" t="n">
+      <c r="N38" s="1" t="n">
         <v>5.5</v>
       </c>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
@@ -4782,8 +4687,6 @@
       <c r="F39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
@@ -4807,17 +4710,15 @@
       <c r="G40" s="1" t="n">
         <v>92.04438506</v>
       </c>
-      <c r="L40" s="0" t="n">
+      <c r="L40" s="1" t="n">
         <v>36.75</v>
       </c>
-      <c r="M40" s="0" t="n">
+      <c r="M40" s="1" t="n">
         <v>5.19272910911395</v>
       </c>
-      <c r="N40" s="0" t="n">
+      <c r="N40" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
@@ -4838,8 +4739,6 @@
       <c r="F41" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
@@ -4869,17 +4768,15 @@
       <c r="K42" s="1" t="n">
         <v>314.713043550195</v>
       </c>
-      <c r="L42" s="0" t="n">
+      <c r="L42" s="1" t="n">
         <v>12.5</v>
       </c>
-      <c r="M42" s="0" t="n">
+      <c r="M42" s="1" t="n">
         <v>0.78705506000237</v>
       </c>
-      <c r="N42" s="0" t="n">
+      <c r="N42" s="1" t="n">
         <v>5.25</v>
       </c>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
@@ -4900,8 +4797,6 @@
       <c r="F43" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
@@ -4925,17 +4820,15 @@
       <c r="G44" s="1" t="n">
         <v>111.1657614</v>
       </c>
-      <c r="L44" s="0" t="n">
+      <c r="L44" s="1" t="n">
         <v>31.75</v>
       </c>
-      <c r="M44" s="0" t="n">
+      <c r="M44" s="1" t="n">
         <v>5.34547264882479</v>
       </c>
-      <c r="N44" s="0" t="n">
+      <c r="N44" s="1" t="n">
         <v>3.25</v>
       </c>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
@@ -4989,13 +4882,13 @@
       <c r="G46" s="1" t="n">
         <v>56.4248001</v>
       </c>
-      <c r="L46" s="0" t="n">
+      <c r="L46" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="M46" s="0" t="n">
+      <c r="M46" s="1" t="n">
         <v>1.63707452480493</v>
       </c>
-      <c r="N46" s="0" t="n">
+      <c r="N46" s="1" t="n">
         <v>3.5</v>
       </c>
       <c r="O46" s="2" t="n">
@@ -5054,8 +4947,6 @@
       <c r="F48" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
@@ -5076,8 +4967,6 @@
       <c r="F49" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
@@ -5101,17 +4990,15 @@
       <c r="G50" s="1" t="n">
         <v>139.1207513</v>
       </c>
-      <c r="L50" s="0" t="n">
+      <c r="L50" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="M50" s="0" t="n">
+      <c r="M50" s="1" t="n">
         <v>3.87231089521166</v>
       </c>
-      <c r="N50" s="0" t="n">
+      <c r="N50" s="1" t="n">
         <v>5.25</v>
       </c>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
@@ -5171,17 +5058,15 @@
       <c r="K52" s="1" t="n">
         <v>510.117646938796</v>
       </c>
-      <c r="L52" s="0" t="n">
+      <c r="L52" s="1" t="n">
         <v>41.75</v>
       </c>
-      <c r="M52" s="0" t="n">
+      <c r="M52" s="1" t="n">
         <v>2.62876390040791</v>
       </c>
-      <c r="N52" s="0" t="n">
+      <c r="N52" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -5247,6 +5132,9 @@
       <c r="I54" s="1" t="n">
         <v>39.36946586</v>
       </c>
+      <c r="J54" s="1" t="n">
+        <v>140.9252211</v>
+      </c>
       <c r="O54" s="2" t="n">
         <v>8.0633</v>
       </c>
@@ -5279,6 +5167,9 @@
       <c r="I55" s="1" t="n">
         <v>11.90918431</v>
       </c>
+      <c r="J55" s="1" t="n">
+        <v>77.00241222</v>
+      </c>
       <c r="O55" s="2" t="n">
         <v>8.776</v>
       </c>
@@ -5337,8 +5228,6 @@
       <c r="G57" s="1" t="n">
         <v>79.71774684</v>
       </c>
-      <c r="O57" s="1"/>
-      <c r="P57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
@@ -5359,8 +5248,6 @@
       <c r="F58" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
@@ -5384,8 +5271,6 @@
       <c r="G59" s="1" t="n">
         <v>61.53991313</v>
       </c>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
@@ -5439,8 +5324,6 @@
       <c r="G61" s="1" t="n">
         <v>40.90035685</v>
       </c>
-      <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
@@ -5461,8 +5344,6 @@
       <c r="F62" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
@@ -5486,8 +5367,6 @@
       <c r="G63" s="1" t="n">
         <v>16.13711754</v>
       </c>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
@@ -5550,7 +5429,6 @@
         <v>23</v>
       </c>
       <c r="O65" s="2"/>
-      <c r="P65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
@@ -5637,8 +5515,6 @@
       <c r="G68" s="1" t="n">
         <v>64.57753223</v>
       </c>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
@@ -5692,3408 +5568,6 @@
       <c r="F70" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O76" s="1"/>
-      <c r="P76" s="1"/>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O77" s="1"/>
-      <c r="P77" s="1"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O78" s="1"/>
-      <c r="P78" s="1"/>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O79" s="1"/>
-      <c r="P79" s="1"/>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O80" s="1"/>
-      <c r="P80" s="1"/>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O81" s="1"/>
-      <c r="P81" s="1"/>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O82" s="1"/>
-      <c r="P82" s="1"/>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O83" s="1"/>
-      <c r="P83" s="1"/>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O84" s="1"/>
-      <c r="P84" s="1"/>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O85" s="1"/>
-      <c r="P85" s="1"/>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O86" s="1"/>
-      <c r="P86" s="1"/>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O87" s="1"/>
-      <c r="P87" s="1"/>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O88" s="1"/>
-      <c r="P88" s="1"/>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O89" s="1"/>
-      <c r="P89" s="1"/>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O90" s="1"/>
-      <c r="P90" s="1"/>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O91" s="1"/>
-      <c r="P91" s="1"/>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O92" s="1"/>
-      <c r="P92" s="1"/>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O93" s="1"/>
-      <c r="P93" s="1"/>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O94" s="1"/>
-      <c r="P94" s="1"/>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O95" s="1"/>
-      <c r="P95" s="1"/>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O96" s="1"/>
-      <c r="P96" s="1"/>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O97" s="1"/>
-      <c r="P97" s="1"/>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O98" s="1"/>
-      <c r="P98" s="1"/>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O99" s="1"/>
-      <c r="P99" s="1"/>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O100" s="1"/>
-      <c r="P100" s="1"/>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O101" s="1"/>
-      <c r="P101" s="1"/>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O102" s="1"/>
-      <c r="P102" s="1"/>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O103" s="1"/>
-      <c r="P103" s="1"/>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O104" s="1"/>
-      <c r="P104" s="1"/>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O105" s="1"/>
-      <c r="P105" s="1"/>
-    </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O106" s="1"/>
-      <c r="P106" s="1"/>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O107" s="1"/>
-      <c r="P107" s="1"/>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O108" s="1"/>
-      <c r="P108" s="1"/>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O109" s="1"/>
-      <c r="P109" s="1"/>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O110" s="1"/>
-      <c r="P110" s="1"/>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O111" s="1"/>
-      <c r="P111" s="1"/>
-    </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O112" s="1"/>
-      <c r="P112" s="1"/>
-    </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O113" s="1"/>
-      <c r="P113" s="1"/>
-    </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O114" s="1"/>
-      <c r="P114" s="1"/>
-    </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O115" s="1"/>
-      <c r="P115" s="1"/>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O116" s="1"/>
-      <c r="P116" s="1"/>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O117" s="1"/>
-      <c r="P117" s="1"/>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O118" s="1"/>
-      <c r="P118" s="1"/>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O119" s="1"/>
-      <c r="P119" s="1"/>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O120" s="1"/>
-      <c r="P120" s="1"/>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O121" s="1"/>
-      <c r="P121" s="1"/>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O122" s="1"/>
-      <c r="P122" s="1"/>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O123" s="1"/>
-      <c r="P123" s="1"/>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O124" s="1"/>
-      <c r="P124" s="1"/>
-    </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O125" s="1"/>
-      <c r="P125" s="1"/>
-    </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O126" s="1"/>
-      <c r="P126" s="1"/>
-    </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O127" s="1"/>
-      <c r="P127" s="1"/>
-    </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O128" s="1"/>
-      <c r="P128" s="1"/>
-    </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O129" s="1"/>
-      <c r="P129" s="1"/>
-    </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O130" s="1"/>
-      <c r="P130" s="1"/>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O131" s="1"/>
-      <c r="P131" s="1"/>
-    </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O132" s="1"/>
-      <c r="P132" s="1"/>
-    </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O133" s="1"/>
-      <c r="P133" s="1"/>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O134" s="1"/>
-      <c r="P134" s="1"/>
-    </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O135" s="1"/>
-      <c r="P135" s="1"/>
-    </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O136" s="1"/>
-      <c r="P136" s="1"/>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O137" s="1"/>
-      <c r="P137" s="1"/>
-    </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O138" s="1"/>
-      <c r="P138" s="1"/>
-    </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O139" s="1"/>
-      <c r="P139" s="1"/>
-    </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O140" s="1"/>
-      <c r="P140" s="1"/>
-    </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O141" s="1"/>
-      <c r="P141" s="1"/>
-    </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O142" s="1"/>
-      <c r="P142" s="1"/>
-    </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O143" s="1"/>
-      <c r="P143" s="1"/>
-    </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O144" s="1"/>
-      <c r="P144" s="1"/>
-    </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O145" s="1"/>
-      <c r="P145" s="1"/>
-    </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O146" s="1"/>
-      <c r="P146" s="1"/>
-    </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O147" s="1"/>
-      <c r="P147" s="1"/>
-    </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O148" s="1"/>
-      <c r="P148" s="1"/>
-    </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O149" s="1"/>
-      <c r="P149" s="1"/>
-    </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O150" s="1"/>
-      <c r="P150" s="1"/>
-    </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O151" s="1"/>
-      <c r="P151" s="1"/>
-    </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O152" s="1"/>
-      <c r="P152" s="1"/>
-    </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O153" s="1"/>
-      <c r="P153" s="1"/>
-    </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O154" s="1"/>
-      <c r="P154" s="1"/>
-    </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O155" s="1"/>
-      <c r="P155" s="1"/>
-    </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O156" s="1"/>
-      <c r="P156" s="1"/>
-    </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O157" s="1"/>
-      <c r="P157" s="1"/>
-    </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O158" s="1"/>
-      <c r="P158" s="1"/>
-    </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O159" s="1"/>
-      <c r="P159" s="1"/>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O160" s="1"/>
-      <c r="P160" s="1"/>
-    </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O161" s="1"/>
-      <c r="P161" s="1"/>
-    </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O162" s="1"/>
-      <c r="P162" s="1"/>
-    </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O163" s="1"/>
-      <c r="P163" s="1"/>
-    </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O164" s="1"/>
-      <c r="P164" s="1"/>
-    </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O165" s="1"/>
-      <c r="P165" s="1"/>
-    </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O166" s="1"/>
-      <c r="P166" s="1"/>
-    </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O167" s="1"/>
-      <c r="P167" s="1"/>
-    </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O168" s="1"/>
-      <c r="P168" s="1"/>
-    </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O169" s="1"/>
-      <c r="P169" s="1"/>
-    </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O170" s="1"/>
-      <c r="P170" s="1"/>
-    </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O171" s="1"/>
-      <c r="P171" s="1"/>
-    </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O172" s="1"/>
-      <c r="P172" s="1"/>
-    </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O173" s="1"/>
-      <c r="P173" s="1"/>
-    </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O174" s="1"/>
-      <c r="P174" s="1"/>
-    </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O175" s="1"/>
-      <c r="P175" s="1"/>
-    </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O176" s="1"/>
-      <c r="P176" s="1"/>
-    </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O177" s="1"/>
-      <c r="P177" s="1"/>
-    </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O178" s="1"/>
-      <c r="P178" s="1"/>
-    </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O179" s="1"/>
-      <c r="P179" s="1"/>
-    </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O180" s="1"/>
-      <c r="P180" s="1"/>
-    </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O181" s="1"/>
-      <c r="P181" s="1"/>
-    </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O182" s="1"/>
-      <c r="P182" s="1"/>
-    </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O183" s="1"/>
-      <c r="P183" s="1"/>
-    </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O184" s="1"/>
-      <c r="P184" s="1"/>
-    </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O185" s="1"/>
-      <c r="P185" s="1"/>
-    </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O186" s="1"/>
-      <c r="P186" s="1"/>
-    </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O187" s="1"/>
-      <c r="P187" s="1"/>
-    </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O188" s="1"/>
-      <c r="P188" s="1"/>
-    </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O189" s="1"/>
-      <c r="P189" s="1"/>
-    </row>
-    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O190" s="1"/>
-      <c r="P190" s="1"/>
-    </row>
-    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O191" s="1"/>
-      <c r="P191" s="1"/>
-    </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O192" s="1"/>
-      <c r="P192" s="1"/>
-    </row>
-    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O193" s="1"/>
-      <c r="P193" s="1"/>
-    </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O194" s="1"/>
-      <c r="P194" s="1"/>
-    </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O195" s="1"/>
-      <c r="P195" s="1"/>
-    </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O196" s="1"/>
-      <c r="P196" s="1"/>
-    </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O197" s="1"/>
-      <c r="P197" s="1"/>
-    </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O198" s="1"/>
-      <c r="P198" s="1"/>
-    </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O199" s="1"/>
-      <c r="P199" s="1"/>
-    </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O200" s="1"/>
-      <c r="P200" s="1"/>
-    </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O201" s="1"/>
-      <c r="P201" s="1"/>
-    </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O202" s="1"/>
-      <c r="P202" s="1"/>
-    </row>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O203" s="1"/>
-      <c r="P203" s="1"/>
-    </row>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O204" s="1"/>
-      <c r="P204" s="1"/>
-    </row>
-    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O205" s="1"/>
-      <c r="P205" s="1"/>
-    </row>
-    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O206" s="1"/>
-      <c r="P206" s="1"/>
-    </row>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O207" s="1"/>
-      <c r="P207" s="1"/>
-    </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O208" s="1"/>
-      <c r="P208" s="1"/>
-    </row>
-    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O209" s="1"/>
-      <c r="P209" s="1"/>
-    </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O210" s="1"/>
-      <c r="P210" s="1"/>
-    </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O211" s="1"/>
-      <c r="P211" s="1"/>
-    </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O212" s="1"/>
-      <c r="P212" s="1"/>
-    </row>
-    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O213" s="1"/>
-      <c r="P213" s="1"/>
-    </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O214" s="1"/>
-      <c r="P214" s="1"/>
-    </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O215" s="1"/>
-      <c r="P215" s="1"/>
-    </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O216" s="1"/>
-      <c r="P216" s="1"/>
-    </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O217" s="1"/>
-      <c r="P217" s="1"/>
-    </row>
-    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O218" s="1"/>
-      <c r="P218" s="1"/>
-    </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O219" s="1"/>
-      <c r="P219" s="1"/>
-    </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O220" s="1"/>
-      <c r="P220" s="1"/>
-    </row>
-    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O221" s="1"/>
-      <c r="P221" s="1"/>
-    </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O222" s="1"/>
-      <c r="P222" s="1"/>
-    </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O223" s="1"/>
-      <c r="P223" s="1"/>
-    </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O224" s="1"/>
-      <c r="P224" s="1"/>
-    </row>
-    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O225" s="1"/>
-      <c r="P225" s="1"/>
-    </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O226" s="1"/>
-      <c r="P226" s="1"/>
-    </row>
-    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O227" s="1"/>
-      <c r="P227" s="1"/>
-    </row>
-    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O228" s="1"/>
-      <c r="P228" s="1"/>
-    </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O229" s="1"/>
-      <c r="P229" s="1"/>
-    </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O230" s="1"/>
-      <c r="P230" s="1"/>
-    </row>
-    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O231" s="1"/>
-      <c r="P231" s="1"/>
-    </row>
-    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O232" s="1"/>
-      <c r="P232" s="1"/>
-    </row>
-    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O233" s="1"/>
-      <c r="P233" s="1"/>
-    </row>
-    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O234" s="1"/>
-      <c r="P234" s="1"/>
-    </row>
-    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O235" s="1"/>
-      <c r="P235" s="1"/>
-    </row>
-    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O236" s="1"/>
-      <c r="P236" s="1"/>
-    </row>
-    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O237" s="1"/>
-      <c r="P237" s="1"/>
-    </row>
-    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O238" s="1"/>
-      <c r="P238" s="1"/>
-    </row>
-    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O239" s="1"/>
-      <c r="P239" s="1"/>
-    </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O240" s="1"/>
-      <c r="P240" s="1"/>
-    </row>
-    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O241" s="1"/>
-      <c r="P241" s="1"/>
-    </row>
-    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O242" s="1"/>
-      <c r="P242" s="1"/>
-    </row>
-    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O243" s="1"/>
-      <c r="P243" s="1"/>
-    </row>
-    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O244" s="1"/>
-      <c r="P244" s="1"/>
-    </row>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O245" s="1"/>
-      <c r="P245" s="1"/>
-    </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O246" s="1"/>
-      <c r="P246" s="1"/>
-    </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O247" s="1"/>
-      <c r="P247" s="1"/>
-    </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O248" s="1"/>
-      <c r="P248" s="1"/>
-    </row>
-    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O249" s="1"/>
-      <c r="P249" s="1"/>
-    </row>
-    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O250" s="1"/>
-      <c r="P250" s="1"/>
-    </row>
-    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O251" s="1"/>
-      <c r="P251" s="1"/>
-    </row>
-    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O252" s="1"/>
-      <c r="P252" s="1"/>
-    </row>
-    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O253" s="1"/>
-      <c r="P253" s="1"/>
-    </row>
-    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O254" s="1"/>
-      <c r="P254" s="1"/>
-    </row>
-    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O255" s="1"/>
-      <c r="P255" s="1"/>
-    </row>
-    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O256" s="1"/>
-      <c r="P256" s="1"/>
-    </row>
-    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O257" s="1"/>
-      <c r="P257" s="1"/>
-    </row>
-    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O258" s="1"/>
-      <c r="P258" s="1"/>
-    </row>
-    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O259" s="1"/>
-      <c r="P259" s="1"/>
-    </row>
-    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O260" s="1"/>
-      <c r="P260" s="1"/>
-    </row>
-    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O261" s="1"/>
-      <c r="P261" s="1"/>
-    </row>
-    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O262" s="1"/>
-      <c r="P262" s="1"/>
-    </row>
-    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O263" s="1"/>
-      <c r="P263" s="1"/>
-    </row>
-    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O264" s="1"/>
-      <c r="P264" s="1"/>
-    </row>
-    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O265" s="1"/>
-      <c r="P265" s="1"/>
-    </row>
-    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O266" s="1"/>
-      <c r="P266" s="1"/>
-    </row>
-    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O267" s="1"/>
-      <c r="P267" s="1"/>
-    </row>
-    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O268" s="1"/>
-      <c r="P268" s="1"/>
-    </row>
-    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O269" s="1"/>
-      <c r="P269" s="1"/>
-    </row>
-    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O270" s="1"/>
-      <c r="P270" s="1"/>
-    </row>
-    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O271" s="1"/>
-      <c r="P271" s="1"/>
-    </row>
-    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O272" s="1"/>
-      <c r="P272" s="1"/>
-    </row>
-    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O273" s="1"/>
-      <c r="P273" s="1"/>
-    </row>
-    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O274" s="1"/>
-      <c r="P274" s="1"/>
-    </row>
-    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O275" s="1"/>
-      <c r="P275" s="1"/>
-    </row>
-    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O276" s="1"/>
-      <c r="P276" s="1"/>
-    </row>
-    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O277" s="1"/>
-      <c r="P277" s="1"/>
-    </row>
-    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O278" s="1"/>
-      <c r="P278" s="1"/>
-    </row>
-    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O279" s="1"/>
-      <c r="P279" s="1"/>
-    </row>
-    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O280" s="1"/>
-      <c r="P280" s="1"/>
-    </row>
-    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O281" s="1"/>
-      <c r="P281" s="1"/>
-    </row>
-    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O282" s="1"/>
-      <c r="P282" s="1"/>
-    </row>
-    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O283" s="1"/>
-      <c r="P283" s="1"/>
-    </row>
-    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O284" s="1"/>
-      <c r="P284" s="1"/>
-    </row>
-    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O285" s="1"/>
-      <c r="P285" s="1"/>
-    </row>
-    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O286" s="1"/>
-      <c r="P286" s="1"/>
-    </row>
-    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O287" s="1"/>
-      <c r="P287" s="1"/>
-    </row>
-    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O288" s="1"/>
-      <c r="P288" s="1"/>
-    </row>
-    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O289" s="1"/>
-      <c r="P289" s="1"/>
-    </row>
-    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O290" s="1"/>
-      <c r="P290" s="1"/>
-    </row>
-    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O291" s="1"/>
-      <c r="P291" s="1"/>
-    </row>
-    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O292" s="1"/>
-      <c r="P292" s="1"/>
-    </row>
-    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O293" s="1"/>
-      <c r="P293" s="1"/>
-    </row>
-    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O294" s="1"/>
-      <c r="P294" s="1"/>
-    </row>
-    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O295" s="1"/>
-      <c r="P295" s="1"/>
-    </row>
-    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O296" s="1"/>
-      <c r="P296" s="1"/>
-    </row>
-    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O297" s="1"/>
-      <c r="P297" s="1"/>
-    </row>
-    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O298" s="1"/>
-      <c r="P298" s="1"/>
-    </row>
-    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O299" s="1"/>
-      <c r="P299" s="1"/>
-    </row>
-    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O300" s="1"/>
-      <c r="P300" s="1"/>
-    </row>
-    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O301" s="1"/>
-      <c r="P301" s="1"/>
-    </row>
-    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O302" s="1"/>
-      <c r="P302" s="1"/>
-    </row>
-    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O303" s="1"/>
-      <c r="P303" s="1"/>
-    </row>
-    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O304" s="1"/>
-      <c r="P304" s="1"/>
-    </row>
-    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O305" s="1"/>
-      <c r="P305" s="1"/>
-    </row>
-    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O306" s="1"/>
-      <c r="P306" s="1"/>
-    </row>
-    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O307" s="1"/>
-      <c r="P307" s="1"/>
-    </row>
-    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O308" s="1"/>
-      <c r="P308" s="1"/>
-    </row>
-    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O309" s="1"/>
-      <c r="P309" s="1"/>
-    </row>
-    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O310" s="1"/>
-      <c r="P310" s="1"/>
-    </row>
-    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O311" s="1"/>
-      <c r="P311" s="1"/>
-    </row>
-    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O312" s="1"/>
-      <c r="P312" s="1"/>
-    </row>
-    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O313" s="1"/>
-      <c r="P313" s="1"/>
-    </row>
-    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O314" s="1"/>
-      <c r="P314" s="1"/>
-    </row>
-    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O315" s="1"/>
-      <c r="P315" s="1"/>
-    </row>
-    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O316" s="1"/>
-      <c r="P316" s="1"/>
-    </row>
-    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O317" s="1"/>
-      <c r="P317" s="1"/>
-    </row>
-    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O318" s="1"/>
-      <c r="P318" s="1"/>
-    </row>
-    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O319" s="1"/>
-      <c r="P319" s="1"/>
-    </row>
-    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O320" s="1"/>
-      <c r="P320" s="1"/>
-    </row>
-    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O321" s="1"/>
-      <c r="P321" s="1"/>
-    </row>
-    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O322" s="1"/>
-      <c r="P322" s="1"/>
-    </row>
-    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O323" s="1"/>
-      <c r="P323" s="1"/>
-    </row>
-    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O324" s="1"/>
-      <c r="P324" s="1"/>
-    </row>
-    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O325" s="1"/>
-      <c r="P325" s="1"/>
-    </row>
-    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O326" s="1"/>
-      <c r="P326" s="1"/>
-    </row>
-    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O327" s="1"/>
-      <c r="P327" s="1"/>
-    </row>
-    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O328" s="1"/>
-      <c r="P328" s="1"/>
-    </row>
-    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O329" s="1"/>
-      <c r="P329" s="1"/>
-    </row>
-    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O330" s="1"/>
-      <c r="P330" s="1"/>
-    </row>
-    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O331" s="1"/>
-      <c r="P331" s="1"/>
-    </row>
-    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O332" s="1"/>
-      <c r="P332" s="1"/>
-    </row>
-    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O333" s="1"/>
-      <c r="P333" s="1"/>
-    </row>
-    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O334" s="1"/>
-      <c r="P334" s="1"/>
-    </row>
-    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O335" s="1"/>
-      <c r="P335" s="1"/>
-    </row>
-    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O336" s="1"/>
-      <c r="P336" s="1"/>
-    </row>
-    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O337" s="1"/>
-      <c r="P337" s="1"/>
-    </row>
-    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O338" s="1"/>
-      <c r="P338" s="1"/>
-    </row>
-    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O339" s="1"/>
-      <c r="P339" s="1"/>
-    </row>
-    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O340" s="1"/>
-      <c r="P340" s="1"/>
-    </row>
-    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O341" s="1"/>
-      <c r="P341" s="1"/>
-    </row>
-    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O342" s="1"/>
-      <c r="P342" s="1"/>
-    </row>
-    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O343" s="1"/>
-      <c r="P343" s="1"/>
-    </row>
-    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O344" s="1"/>
-      <c r="P344" s="1"/>
-    </row>
-    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O345" s="1"/>
-      <c r="P345" s="1"/>
-    </row>
-    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O346" s="1"/>
-      <c r="P346" s="1"/>
-    </row>
-    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O347" s="1"/>
-      <c r="P347" s="1"/>
-    </row>
-    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O348" s="1"/>
-      <c r="P348" s="1"/>
-    </row>
-    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O349" s="1"/>
-      <c r="P349" s="1"/>
-    </row>
-    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O350" s="1"/>
-      <c r="P350" s="1"/>
-    </row>
-    <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O351" s="1"/>
-      <c r="P351" s="1"/>
-    </row>
-    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O352" s="1"/>
-      <c r="P352" s="1"/>
-    </row>
-    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O353" s="1"/>
-      <c r="P353" s="1"/>
-    </row>
-    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O354" s="1"/>
-      <c r="P354" s="1"/>
-    </row>
-    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O355" s="1"/>
-      <c r="P355" s="1"/>
-    </row>
-    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O356" s="1"/>
-      <c r="P356" s="1"/>
-    </row>
-    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O357" s="1"/>
-      <c r="P357" s="1"/>
-    </row>
-    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O358" s="1"/>
-      <c r="P358" s="1"/>
-    </row>
-    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O359" s="1"/>
-      <c r="P359" s="1"/>
-    </row>
-    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O360" s="1"/>
-      <c r="P360" s="1"/>
-    </row>
-    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O361" s="1"/>
-      <c r="P361" s="1"/>
-    </row>
-    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O362" s="1"/>
-      <c r="P362" s="1"/>
-    </row>
-    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O363" s="1"/>
-      <c r="P363" s="1"/>
-    </row>
-    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O364" s="1"/>
-      <c r="P364" s="1"/>
-    </row>
-    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O365" s="1"/>
-      <c r="P365" s="1"/>
-    </row>
-    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O366" s="1"/>
-      <c r="P366" s="1"/>
-    </row>
-    <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O367" s="1"/>
-      <c r="P367" s="1"/>
-    </row>
-    <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O368" s="1"/>
-      <c r="P368" s="1"/>
-    </row>
-    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O369" s="1"/>
-      <c r="P369" s="1"/>
-    </row>
-    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O370" s="1"/>
-      <c r="P370" s="1"/>
-    </row>
-    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O371" s="1"/>
-      <c r="P371" s="1"/>
-    </row>
-    <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O372" s="1"/>
-      <c r="P372" s="1"/>
-    </row>
-    <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O373" s="1"/>
-      <c r="P373" s="1"/>
-    </row>
-    <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O374" s="1"/>
-      <c r="P374" s="1"/>
-    </row>
-    <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O375" s="1"/>
-      <c r="P375" s="1"/>
-    </row>
-    <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O376" s="1"/>
-      <c r="P376" s="1"/>
-    </row>
-    <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O377" s="1"/>
-      <c r="P377" s="1"/>
-    </row>
-    <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O378" s="1"/>
-      <c r="P378" s="1"/>
-    </row>
-    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O379" s="1"/>
-      <c r="P379" s="1"/>
-    </row>
-    <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O380" s="1"/>
-      <c r="P380" s="1"/>
-    </row>
-    <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O381" s="1"/>
-      <c r="P381" s="1"/>
-    </row>
-    <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O382" s="1"/>
-      <c r="P382" s="1"/>
-    </row>
-    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O383" s="1"/>
-      <c r="P383" s="1"/>
-    </row>
-    <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O384" s="1"/>
-      <c r="P384" s="1"/>
-    </row>
-    <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O385" s="1"/>
-      <c r="P385" s="1"/>
-    </row>
-    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O386" s="1"/>
-      <c r="P386" s="1"/>
-    </row>
-    <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O387" s="1"/>
-      <c r="P387" s="1"/>
-    </row>
-    <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O388" s="1"/>
-      <c r="P388" s="1"/>
-    </row>
-    <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O389" s="1"/>
-      <c r="P389" s="1"/>
-    </row>
-    <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O390" s="1"/>
-      <c r="P390" s="1"/>
-    </row>
-    <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O391" s="1"/>
-      <c r="P391" s="1"/>
-    </row>
-    <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O392" s="1"/>
-      <c r="P392" s="1"/>
-    </row>
-    <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O393" s="1"/>
-      <c r="P393" s="1"/>
-    </row>
-    <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O394" s="1"/>
-      <c r="P394" s="1"/>
-    </row>
-    <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O395" s="1"/>
-      <c r="P395" s="1"/>
-    </row>
-    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O396" s="1"/>
-      <c r="P396" s="1"/>
-    </row>
-    <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O397" s="1"/>
-      <c r="P397" s="1"/>
-    </row>
-    <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O398" s="1"/>
-      <c r="P398" s="1"/>
-    </row>
-    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O399" s="1"/>
-      <c r="P399" s="1"/>
-    </row>
-    <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O400" s="1"/>
-      <c r="P400" s="1"/>
-    </row>
-    <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O401" s="1"/>
-      <c r="P401" s="1"/>
-    </row>
-    <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O402" s="1"/>
-      <c r="P402" s="1"/>
-    </row>
-    <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O403" s="1"/>
-      <c r="P403" s="1"/>
-    </row>
-    <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O404" s="1"/>
-      <c r="P404" s="1"/>
-    </row>
-    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O405" s="1"/>
-      <c r="P405" s="1"/>
-    </row>
-    <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O406" s="1"/>
-      <c r="P406" s="1"/>
-    </row>
-    <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O407" s="1"/>
-      <c r="P407" s="1"/>
-    </row>
-    <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O408" s="1"/>
-      <c r="P408" s="1"/>
-    </row>
-    <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O409" s="1"/>
-      <c r="P409" s="1"/>
-    </row>
-    <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O410" s="1"/>
-      <c r="P410" s="1"/>
-    </row>
-    <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O411" s="1"/>
-      <c r="P411" s="1"/>
-    </row>
-    <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O412" s="1"/>
-      <c r="P412" s="1"/>
-    </row>
-    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O413" s="1"/>
-      <c r="P413" s="1"/>
-    </row>
-    <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O414" s="1"/>
-      <c r="P414" s="1"/>
-    </row>
-    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O415" s="1"/>
-      <c r="P415" s="1"/>
-    </row>
-    <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O416" s="1"/>
-      <c r="P416" s="1"/>
-    </row>
-    <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O417" s="1"/>
-      <c r="P417" s="1"/>
-    </row>
-    <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O418" s="1"/>
-      <c r="P418" s="1"/>
-    </row>
-    <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O419" s="1"/>
-      <c r="P419" s="1"/>
-    </row>
-    <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O420" s="1"/>
-      <c r="P420" s="1"/>
-    </row>
-    <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O421" s="1"/>
-      <c r="P421" s="1"/>
-    </row>
-    <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O422" s="1"/>
-      <c r="P422" s="1"/>
-    </row>
-    <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O423" s="1"/>
-      <c r="P423" s="1"/>
-    </row>
-    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O424" s="1"/>
-      <c r="P424" s="1"/>
-    </row>
-    <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O425" s="1"/>
-      <c r="P425" s="1"/>
-    </row>
-    <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O426" s="1"/>
-      <c r="P426" s="1"/>
-    </row>
-    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O427" s="1"/>
-      <c r="P427" s="1"/>
-    </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O428" s="1"/>
-      <c r="P428" s="1"/>
-    </row>
-    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O429" s="1"/>
-      <c r="P429" s="1"/>
-    </row>
-    <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O430" s="1"/>
-      <c r="P430" s="1"/>
-    </row>
-    <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O431" s="1"/>
-      <c r="P431" s="1"/>
-    </row>
-    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O432" s="1"/>
-      <c r="P432" s="1"/>
-    </row>
-    <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O433" s="1"/>
-      <c r="P433" s="1"/>
-    </row>
-    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O434" s="1"/>
-      <c r="P434" s="1"/>
-    </row>
-    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O435" s="1"/>
-      <c r="P435" s="1"/>
-    </row>
-    <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O436" s="1"/>
-      <c r="P436" s="1"/>
-    </row>
-    <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O437" s="1"/>
-      <c r="P437" s="1"/>
-    </row>
-    <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O438" s="1"/>
-      <c r="P438" s="1"/>
-    </row>
-    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O439" s="1"/>
-      <c r="P439" s="1"/>
-    </row>
-    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O440" s="1"/>
-      <c r="P440" s="1"/>
-    </row>
-    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O441" s="1"/>
-      <c r="P441" s="1"/>
-    </row>
-    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O442" s="1"/>
-      <c r="P442" s="1"/>
-    </row>
-    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O443" s="1"/>
-      <c r="P443" s="1"/>
-    </row>
-    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O444" s="1"/>
-      <c r="P444" s="1"/>
-    </row>
-    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O445" s="1"/>
-      <c r="P445" s="1"/>
-    </row>
-    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O446" s="1"/>
-      <c r="P446" s="1"/>
-    </row>
-    <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O447" s="1"/>
-      <c r="P447" s="1"/>
-    </row>
-    <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O448" s="1"/>
-      <c r="P448" s="1"/>
-    </row>
-    <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O449" s="1"/>
-      <c r="P449" s="1"/>
-    </row>
-    <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O450" s="1"/>
-      <c r="P450" s="1"/>
-    </row>
-    <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O451" s="1"/>
-      <c r="P451" s="1"/>
-    </row>
-    <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O452" s="1"/>
-      <c r="P452" s="1"/>
-    </row>
-    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O453" s="1"/>
-      <c r="P453" s="1"/>
-    </row>
-    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O454" s="1"/>
-      <c r="P454" s="1"/>
-    </row>
-    <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O455" s="1"/>
-      <c r="P455" s="1"/>
-    </row>
-    <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O456" s="1"/>
-      <c r="P456" s="1"/>
-    </row>
-    <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O457" s="1"/>
-      <c r="P457" s="1"/>
-    </row>
-    <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O458" s="1"/>
-      <c r="P458" s="1"/>
-    </row>
-    <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O459" s="1"/>
-      <c r="P459" s="1"/>
-    </row>
-    <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O460" s="1"/>
-      <c r="P460" s="1"/>
-    </row>
-    <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O461" s="1"/>
-      <c r="P461" s="1"/>
-    </row>
-    <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O462" s="1"/>
-      <c r="P462" s="1"/>
-    </row>
-    <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O463" s="1"/>
-      <c r="P463" s="1"/>
-    </row>
-    <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O464" s="1"/>
-      <c r="P464" s="1"/>
-    </row>
-    <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O465" s="1"/>
-      <c r="P465" s="1"/>
-    </row>
-    <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O466" s="1"/>
-      <c r="P466" s="1"/>
-    </row>
-    <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O467" s="1"/>
-      <c r="P467" s="1"/>
-    </row>
-    <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O468" s="1"/>
-      <c r="P468" s="1"/>
-    </row>
-    <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O469" s="1"/>
-      <c r="P469" s="1"/>
-    </row>
-    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O470" s="1"/>
-      <c r="P470" s="1"/>
-    </row>
-    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O471" s="1"/>
-      <c r="P471" s="1"/>
-    </row>
-    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O472" s="1"/>
-      <c r="P472" s="1"/>
-    </row>
-    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O473" s="1"/>
-      <c r="P473" s="1"/>
-    </row>
-    <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O474" s="1"/>
-      <c r="P474" s="1"/>
-    </row>
-    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O475" s="1"/>
-      <c r="P475" s="1"/>
-    </row>
-    <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O476" s="1"/>
-      <c r="P476" s="1"/>
-    </row>
-    <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O477" s="1"/>
-      <c r="P477" s="1"/>
-    </row>
-    <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O478" s="1"/>
-      <c r="P478" s="1"/>
-    </row>
-    <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O479" s="1"/>
-      <c r="P479" s="1"/>
-    </row>
-    <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O480" s="1"/>
-      <c r="P480" s="1"/>
-    </row>
-    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O481" s="1"/>
-      <c r="P481" s="1"/>
-    </row>
-    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O482" s="1"/>
-      <c r="P482" s="1"/>
-    </row>
-    <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O483" s="1"/>
-      <c r="P483" s="1"/>
-    </row>
-    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O484" s="1"/>
-      <c r="P484" s="1"/>
-    </row>
-    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O485" s="1"/>
-      <c r="P485" s="1"/>
-    </row>
-    <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O486" s="1"/>
-      <c r="P486" s="1"/>
-    </row>
-    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O487" s="1"/>
-      <c r="P487" s="1"/>
-    </row>
-    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O488" s="1"/>
-      <c r="P488" s="1"/>
-    </row>
-    <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O489" s="1"/>
-      <c r="P489" s="1"/>
-    </row>
-    <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O490" s="1"/>
-      <c r="P490" s="1"/>
-    </row>
-    <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O491" s="1"/>
-      <c r="P491" s="1"/>
-    </row>
-    <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O492" s="1"/>
-      <c r="P492" s="1"/>
-    </row>
-    <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O493" s="1"/>
-      <c r="P493" s="1"/>
-    </row>
-    <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O494" s="1"/>
-      <c r="P494" s="1"/>
-    </row>
-    <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O495" s="1"/>
-      <c r="P495" s="1"/>
-    </row>
-    <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O496" s="1"/>
-      <c r="P496" s="1"/>
-    </row>
-    <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O497" s="1"/>
-      <c r="P497" s="1"/>
-    </row>
-    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O498" s="1"/>
-      <c r="P498" s="1"/>
-    </row>
-    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O499" s="1"/>
-      <c r="P499" s="1"/>
-    </row>
-    <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O500" s="1"/>
-      <c r="P500" s="1"/>
-    </row>
-    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O501" s="1"/>
-      <c r="P501" s="1"/>
-    </row>
-    <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O502" s="1"/>
-      <c r="P502" s="1"/>
-    </row>
-    <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O503" s="1"/>
-      <c r="P503" s="1"/>
-    </row>
-    <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O504" s="1"/>
-      <c r="P504" s="1"/>
-    </row>
-    <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O505" s="1"/>
-      <c r="P505" s="1"/>
-    </row>
-    <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O506" s="1"/>
-      <c r="P506" s="1"/>
-    </row>
-    <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O507" s="1"/>
-      <c r="P507" s="1"/>
-    </row>
-    <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O508" s="1"/>
-      <c r="P508" s="1"/>
-    </row>
-    <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O509" s="1"/>
-      <c r="P509" s="1"/>
-    </row>
-    <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O510" s="1"/>
-      <c r="P510" s="1"/>
-    </row>
-    <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O511" s="1"/>
-      <c r="P511" s="1"/>
-    </row>
-    <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O512" s="1"/>
-      <c r="P512" s="1"/>
-    </row>
-    <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O513" s="1"/>
-      <c r="P513" s="1"/>
-    </row>
-    <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O514" s="1"/>
-      <c r="P514" s="1"/>
-    </row>
-    <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O515" s="1"/>
-      <c r="P515" s="1"/>
-    </row>
-    <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O516" s="1"/>
-      <c r="P516" s="1"/>
-    </row>
-    <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O517" s="1"/>
-      <c r="P517" s="1"/>
-    </row>
-    <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O518" s="1"/>
-      <c r="P518" s="1"/>
-    </row>
-    <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O519" s="1"/>
-      <c r="P519" s="1"/>
-    </row>
-    <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O520" s="1"/>
-      <c r="P520" s="1"/>
-    </row>
-    <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O521" s="1"/>
-      <c r="P521" s="1"/>
-    </row>
-    <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O522" s="1"/>
-      <c r="P522" s="1"/>
-    </row>
-    <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O523" s="1"/>
-      <c r="P523" s="1"/>
-    </row>
-    <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O524" s="1"/>
-      <c r="P524" s="1"/>
-    </row>
-    <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O525" s="1"/>
-      <c r="P525" s="1"/>
-    </row>
-    <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O526" s="1"/>
-      <c r="P526" s="1"/>
-    </row>
-    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O527" s="1"/>
-      <c r="P527" s="1"/>
-    </row>
-    <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O528" s="1"/>
-      <c r="P528" s="1"/>
-    </row>
-    <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O529" s="1"/>
-      <c r="P529" s="1"/>
-    </row>
-    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O530" s="1"/>
-      <c r="P530" s="1"/>
-    </row>
-    <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O531" s="1"/>
-      <c r="P531" s="1"/>
-    </row>
-    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O532" s="1"/>
-      <c r="P532" s="1"/>
-    </row>
-    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O533" s="1"/>
-      <c r="P533" s="1"/>
-    </row>
-    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O534" s="1"/>
-      <c r="P534" s="1"/>
-    </row>
-    <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O535" s="1"/>
-      <c r="P535" s="1"/>
-    </row>
-    <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O536" s="1"/>
-      <c r="P536" s="1"/>
-    </row>
-    <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O537" s="1"/>
-      <c r="P537" s="1"/>
-    </row>
-    <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O538" s="1"/>
-      <c r="P538" s="1"/>
-    </row>
-    <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O539" s="1"/>
-      <c r="P539" s="1"/>
-    </row>
-    <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O540" s="1"/>
-      <c r="P540" s="1"/>
-    </row>
-    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O541" s="1"/>
-      <c r="P541" s="1"/>
-    </row>
-    <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O542" s="1"/>
-      <c r="P542" s="1"/>
-    </row>
-    <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O543" s="1"/>
-      <c r="P543" s="1"/>
-    </row>
-    <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O544" s="1"/>
-      <c r="P544" s="1"/>
-    </row>
-    <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O545" s="1"/>
-      <c r="P545" s="1"/>
-    </row>
-    <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O546" s="1"/>
-      <c r="P546" s="1"/>
-    </row>
-    <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O547" s="1"/>
-      <c r="P547" s="1"/>
-    </row>
-    <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O548" s="1"/>
-      <c r="P548" s="1"/>
-    </row>
-    <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O549" s="1"/>
-      <c r="P549" s="1"/>
-    </row>
-    <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O550" s="1"/>
-      <c r="P550" s="1"/>
-    </row>
-    <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O551" s="1"/>
-      <c r="P551" s="1"/>
-    </row>
-    <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O552" s="1"/>
-      <c r="P552" s="1"/>
-    </row>
-    <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O553" s="1"/>
-      <c r="P553" s="1"/>
-    </row>
-    <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O554" s="1"/>
-      <c r="P554" s="1"/>
-    </row>
-    <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O555" s="1"/>
-      <c r="P555" s="1"/>
-    </row>
-    <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O556" s="1"/>
-      <c r="P556" s="1"/>
-    </row>
-    <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O557" s="1"/>
-      <c r="P557" s="1"/>
-    </row>
-    <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O558" s="1"/>
-      <c r="P558" s="1"/>
-    </row>
-    <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O559" s="1"/>
-      <c r="P559" s="1"/>
-    </row>
-    <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O560" s="1"/>
-      <c r="P560" s="1"/>
-    </row>
-    <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O561" s="1"/>
-      <c r="P561" s="1"/>
-    </row>
-    <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O562" s="1"/>
-      <c r="P562" s="1"/>
-    </row>
-    <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O563" s="1"/>
-      <c r="P563" s="1"/>
-    </row>
-    <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O564" s="1"/>
-      <c r="P564" s="1"/>
-    </row>
-    <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O565" s="1"/>
-      <c r="P565" s="1"/>
-    </row>
-    <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O566" s="1"/>
-      <c r="P566" s="1"/>
-    </row>
-    <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O567" s="1"/>
-      <c r="P567" s="1"/>
-    </row>
-    <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O568" s="1"/>
-      <c r="P568" s="1"/>
-    </row>
-    <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O569" s="1"/>
-      <c r="P569" s="1"/>
-    </row>
-    <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O570" s="1"/>
-      <c r="P570" s="1"/>
-    </row>
-    <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O571" s="1"/>
-      <c r="P571" s="1"/>
-    </row>
-    <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O572" s="1"/>
-      <c r="P572" s="1"/>
-    </row>
-    <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O573" s="1"/>
-      <c r="P573" s="1"/>
-    </row>
-    <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O574" s="1"/>
-      <c r="P574" s="1"/>
-    </row>
-    <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O575" s="1"/>
-      <c r="P575" s="1"/>
-    </row>
-    <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O576" s="1"/>
-      <c r="P576" s="1"/>
-    </row>
-    <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O577" s="1"/>
-      <c r="P577" s="1"/>
-    </row>
-    <row r="578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O578" s="1"/>
-      <c r="P578" s="1"/>
-    </row>
-    <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O579" s="1"/>
-      <c r="P579" s="1"/>
-    </row>
-    <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O580" s="1"/>
-      <c r="P580" s="1"/>
-    </row>
-    <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O581" s="1"/>
-      <c r="P581" s="1"/>
-    </row>
-    <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O582" s="1"/>
-      <c r="P582" s="1"/>
-    </row>
-    <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O583" s="1"/>
-      <c r="P583" s="1"/>
-    </row>
-    <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O584" s="1"/>
-      <c r="P584" s="1"/>
-    </row>
-    <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O585" s="1"/>
-      <c r="P585" s="1"/>
-    </row>
-    <row r="586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O586" s="1"/>
-      <c r="P586" s="1"/>
-    </row>
-    <row r="587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O587" s="1"/>
-      <c r="P587" s="1"/>
-    </row>
-    <row r="588" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O588" s="1"/>
-      <c r="P588" s="1"/>
-    </row>
-    <row r="589" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O589" s="1"/>
-      <c r="P589" s="1"/>
-    </row>
-    <row r="590" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O590" s="1"/>
-      <c r="P590" s="1"/>
-    </row>
-    <row r="591" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O591" s="1"/>
-      <c r="P591" s="1"/>
-    </row>
-    <row r="592" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O592" s="1"/>
-      <c r="P592" s="1"/>
-    </row>
-    <row r="593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O593" s="1"/>
-      <c r="P593" s="1"/>
-    </row>
-    <row r="594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O594" s="1"/>
-      <c r="P594" s="1"/>
-    </row>
-    <row r="595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O595" s="1"/>
-      <c r="P595" s="1"/>
-    </row>
-    <row r="596" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O596" s="1"/>
-      <c r="P596" s="1"/>
-    </row>
-    <row r="597" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O597" s="1"/>
-      <c r="P597" s="1"/>
-    </row>
-    <row r="598" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O598" s="1"/>
-      <c r="P598" s="1"/>
-    </row>
-    <row r="599" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O599" s="1"/>
-      <c r="P599" s="1"/>
-    </row>
-    <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O600" s="1"/>
-      <c r="P600" s="1"/>
-    </row>
-    <row r="601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O601" s="1"/>
-      <c r="P601" s="1"/>
-    </row>
-    <row r="602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O602" s="1"/>
-      <c r="P602" s="1"/>
-    </row>
-    <row r="603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O603" s="1"/>
-      <c r="P603" s="1"/>
-    </row>
-    <row r="604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O604" s="1"/>
-      <c r="P604" s="1"/>
-    </row>
-    <row r="605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O605" s="1"/>
-      <c r="P605" s="1"/>
-    </row>
-    <row r="606" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O606" s="1"/>
-      <c r="P606" s="1"/>
-    </row>
-    <row r="607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O607" s="1"/>
-      <c r="P607" s="1"/>
-    </row>
-    <row r="608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O608" s="1"/>
-      <c r="P608" s="1"/>
-    </row>
-    <row r="609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O609" s="1"/>
-      <c r="P609" s="1"/>
-    </row>
-    <row r="610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O610" s="1"/>
-      <c r="P610" s="1"/>
-    </row>
-    <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O611" s="1"/>
-      <c r="P611" s="1"/>
-    </row>
-    <row r="612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O612" s="1"/>
-      <c r="P612" s="1"/>
-    </row>
-    <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O613" s="1"/>
-      <c r="P613" s="1"/>
-    </row>
-    <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O614" s="1"/>
-      <c r="P614" s="1"/>
-    </row>
-    <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O615" s="1"/>
-      <c r="P615" s="1"/>
-    </row>
-    <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O616" s="1"/>
-      <c r="P616" s="1"/>
-    </row>
-    <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O617" s="1"/>
-      <c r="P617" s="1"/>
-    </row>
-    <row r="618" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O618" s="1"/>
-      <c r="P618" s="1"/>
-    </row>
-    <row r="619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O619" s="1"/>
-      <c r="P619" s="1"/>
-    </row>
-    <row r="620" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O620" s="1"/>
-      <c r="P620" s="1"/>
-    </row>
-    <row r="621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O621" s="1"/>
-      <c r="P621" s="1"/>
-    </row>
-    <row r="622" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O622" s="1"/>
-      <c r="P622" s="1"/>
-    </row>
-    <row r="623" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O623" s="1"/>
-      <c r="P623" s="1"/>
-    </row>
-    <row r="624" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O624" s="1"/>
-      <c r="P624" s="1"/>
-    </row>
-    <row r="625" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O625" s="1"/>
-      <c r="P625" s="1"/>
-    </row>
-    <row r="626" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O626" s="1"/>
-      <c r="P626" s="1"/>
-    </row>
-    <row r="627" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O627" s="1"/>
-      <c r="P627" s="1"/>
-    </row>
-    <row r="628" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O628" s="1"/>
-      <c r="P628" s="1"/>
-    </row>
-    <row r="629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O629" s="1"/>
-      <c r="P629" s="1"/>
-    </row>
-    <row r="630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O630" s="1"/>
-      <c r="P630" s="1"/>
-    </row>
-    <row r="631" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O631" s="1"/>
-      <c r="P631" s="1"/>
-    </row>
-    <row r="632" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O632" s="1"/>
-      <c r="P632" s="1"/>
-    </row>
-    <row r="633" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O633" s="1"/>
-      <c r="P633" s="1"/>
-    </row>
-    <row r="634" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O634" s="1"/>
-      <c r="P634" s="1"/>
-    </row>
-    <row r="635" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O635" s="1"/>
-      <c r="P635" s="1"/>
-    </row>
-    <row r="636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O636" s="1"/>
-      <c r="P636" s="1"/>
-    </row>
-    <row r="637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O637" s="1"/>
-      <c r="P637" s="1"/>
-    </row>
-    <row r="638" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O638" s="1"/>
-      <c r="P638" s="1"/>
-    </row>
-    <row r="639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O639" s="1"/>
-      <c r="P639" s="1"/>
-    </row>
-    <row r="640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O640" s="1"/>
-      <c r="P640" s="1"/>
-    </row>
-    <row r="641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O641" s="1"/>
-      <c r="P641" s="1"/>
-    </row>
-    <row r="642" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O642" s="1"/>
-      <c r="P642" s="1"/>
-    </row>
-    <row r="643" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O643" s="1"/>
-      <c r="P643" s="1"/>
-    </row>
-    <row r="644" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O644" s="1"/>
-      <c r="P644" s="1"/>
-    </row>
-    <row r="645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O645" s="1"/>
-      <c r="P645" s="1"/>
-    </row>
-    <row r="646" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O646" s="1"/>
-      <c r="P646" s="1"/>
-    </row>
-    <row r="647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O647" s="1"/>
-      <c r="P647" s="1"/>
-    </row>
-    <row r="648" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O648" s="1"/>
-      <c r="P648" s="1"/>
-    </row>
-    <row r="649" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O649" s="1"/>
-      <c r="P649" s="1"/>
-    </row>
-    <row r="650" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O650" s="1"/>
-      <c r="P650" s="1"/>
-    </row>
-    <row r="651" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O651" s="1"/>
-      <c r="P651" s="1"/>
-    </row>
-    <row r="652" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O652" s="1"/>
-      <c r="P652" s="1"/>
-    </row>
-    <row r="653" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O653" s="1"/>
-      <c r="P653" s="1"/>
-    </row>
-    <row r="654" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O654" s="1"/>
-      <c r="P654" s="1"/>
-    </row>
-    <row r="655" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O655" s="1"/>
-      <c r="P655" s="1"/>
-    </row>
-    <row r="656" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O656" s="1"/>
-      <c r="P656" s="1"/>
-    </row>
-    <row r="657" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O657" s="1"/>
-      <c r="P657" s="1"/>
-    </row>
-    <row r="658" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O658" s="1"/>
-      <c r="P658" s="1"/>
-    </row>
-    <row r="659" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O659" s="1"/>
-      <c r="P659" s="1"/>
-    </row>
-    <row r="660" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O660" s="1"/>
-      <c r="P660" s="1"/>
-    </row>
-    <row r="661" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O661" s="1"/>
-      <c r="P661" s="1"/>
-    </row>
-    <row r="662" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O662" s="1"/>
-      <c r="P662" s="1"/>
-    </row>
-    <row r="663" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O663" s="1"/>
-      <c r="P663" s="1"/>
-    </row>
-    <row r="664" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O664" s="1"/>
-      <c r="P664" s="1"/>
-    </row>
-    <row r="665" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O665" s="1"/>
-      <c r="P665" s="1"/>
-    </row>
-    <row r="666" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O666" s="1"/>
-      <c r="P666" s="1"/>
-    </row>
-    <row r="667" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O667" s="1"/>
-      <c r="P667" s="1"/>
-    </row>
-    <row r="668" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O668" s="1"/>
-      <c r="P668" s="1"/>
-    </row>
-    <row r="669" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O669" s="1"/>
-      <c r="P669" s="1"/>
-    </row>
-    <row r="670" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O670" s="1"/>
-      <c r="P670" s="1"/>
-    </row>
-    <row r="671" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O671" s="1"/>
-      <c r="P671" s="1"/>
-    </row>
-    <row r="672" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O672" s="1"/>
-      <c r="P672" s="1"/>
-    </row>
-    <row r="673" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O673" s="1"/>
-      <c r="P673" s="1"/>
-    </row>
-    <row r="674" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O674" s="1"/>
-      <c r="P674" s="1"/>
-    </row>
-    <row r="675" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O675" s="1"/>
-      <c r="P675" s="1"/>
-    </row>
-    <row r="676" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O676" s="1"/>
-      <c r="P676" s="1"/>
-    </row>
-    <row r="677" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O677" s="1"/>
-      <c r="P677" s="1"/>
-    </row>
-    <row r="678" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O678" s="1"/>
-      <c r="P678" s="1"/>
-    </row>
-    <row r="679" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O679" s="1"/>
-      <c r="P679" s="1"/>
-    </row>
-    <row r="680" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O680" s="1"/>
-      <c r="P680" s="1"/>
-    </row>
-    <row r="681" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O681" s="1"/>
-      <c r="P681" s="1"/>
-    </row>
-    <row r="682" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O682" s="1"/>
-      <c r="P682" s="1"/>
-    </row>
-    <row r="683" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O683" s="1"/>
-      <c r="P683" s="1"/>
-    </row>
-    <row r="684" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O684" s="1"/>
-      <c r="P684" s="1"/>
-    </row>
-    <row r="685" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O685" s="1"/>
-      <c r="P685" s="1"/>
-    </row>
-    <row r="686" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O686" s="1"/>
-      <c r="P686" s="1"/>
-    </row>
-    <row r="687" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O687" s="1"/>
-      <c r="P687" s="1"/>
-    </row>
-    <row r="688" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O688" s="1"/>
-      <c r="P688" s="1"/>
-    </row>
-    <row r="689" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O689" s="1"/>
-      <c r="P689" s="1"/>
-    </row>
-    <row r="690" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O690" s="1"/>
-      <c r="P690" s="1"/>
-    </row>
-    <row r="691" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O691" s="1"/>
-      <c r="P691" s="1"/>
-    </row>
-    <row r="692" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O692" s="1"/>
-      <c r="P692" s="1"/>
-    </row>
-    <row r="693" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O693" s="1"/>
-      <c r="P693" s="1"/>
-    </row>
-    <row r="694" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O694" s="1"/>
-      <c r="P694" s="1"/>
-    </row>
-    <row r="695" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O695" s="1"/>
-      <c r="P695" s="1"/>
-    </row>
-    <row r="696" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O696" s="1"/>
-      <c r="P696" s="1"/>
-    </row>
-    <row r="697" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O697" s="1"/>
-      <c r="P697" s="1"/>
-    </row>
-    <row r="698" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O698" s="1"/>
-      <c r="P698" s="1"/>
-    </row>
-    <row r="699" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O699" s="1"/>
-      <c r="P699" s="1"/>
-    </row>
-    <row r="700" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O700" s="1"/>
-      <c r="P700" s="1"/>
-    </row>
-    <row r="701" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O701" s="1"/>
-      <c r="P701" s="1"/>
-    </row>
-    <row r="702" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O702" s="1"/>
-      <c r="P702" s="1"/>
-    </row>
-    <row r="703" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O703" s="1"/>
-      <c r="P703" s="1"/>
-    </row>
-    <row r="704" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O704" s="1"/>
-      <c r="P704" s="1"/>
-    </row>
-    <row r="705" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O705" s="1"/>
-      <c r="P705" s="1"/>
-    </row>
-    <row r="706" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O706" s="1"/>
-      <c r="P706" s="1"/>
-    </row>
-    <row r="707" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O707" s="1"/>
-      <c r="P707" s="1"/>
-    </row>
-    <row r="708" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O708" s="1"/>
-      <c r="P708" s="1"/>
-    </row>
-    <row r="709" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O709" s="1"/>
-      <c r="P709" s="1"/>
-    </row>
-    <row r="710" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O710" s="1"/>
-      <c r="P710" s="1"/>
-    </row>
-    <row r="711" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O711" s="1"/>
-      <c r="P711" s="1"/>
-    </row>
-    <row r="712" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O712" s="1"/>
-      <c r="P712" s="1"/>
-    </row>
-    <row r="713" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O713" s="1"/>
-      <c r="P713" s="1"/>
-    </row>
-    <row r="714" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O714" s="1"/>
-      <c r="P714" s="1"/>
-    </row>
-    <row r="715" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O715" s="1"/>
-      <c r="P715" s="1"/>
-    </row>
-    <row r="716" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O716" s="1"/>
-      <c r="P716" s="1"/>
-    </row>
-    <row r="717" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O717" s="1"/>
-      <c r="P717" s="1"/>
-    </row>
-    <row r="718" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O718" s="1"/>
-      <c r="P718" s="1"/>
-    </row>
-    <row r="719" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O719" s="1"/>
-      <c r="P719" s="1"/>
-    </row>
-    <row r="720" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O720" s="1"/>
-      <c r="P720" s="1"/>
-    </row>
-    <row r="721" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O721" s="1"/>
-      <c r="P721" s="1"/>
-    </row>
-    <row r="722" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O722" s="1"/>
-      <c r="P722" s="1"/>
-    </row>
-    <row r="723" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O723" s="1"/>
-      <c r="P723" s="1"/>
-    </row>
-    <row r="724" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O724" s="1"/>
-      <c r="P724" s="1"/>
-    </row>
-    <row r="725" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O725" s="1"/>
-      <c r="P725" s="1"/>
-    </row>
-    <row r="726" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O726" s="1"/>
-      <c r="P726" s="1"/>
-    </row>
-    <row r="727" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O727" s="1"/>
-      <c r="P727" s="1"/>
-    </row>
-    <row r="728" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O728" s="1"/>
-      <c r="P728" s="1"/>
-    </row>
-    <row r="729" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O729" s="1"/>
-      <c r="P729" s="1"/>
-    </row>
-    <row r="730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O730" s="1"/>
-      <c r="P730" s="1"/>
-    </row>
-    <row r="731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O731" s="1"/>
-      <c r="P731" s="1"/>
-    </row>
-    <row r="732" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O732" s="1"/>
-      <c r="P732" s="1"/>
-    </row>
-    <row r="733" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O733" s="1"/>
-      <c r="P733" s="1"/>
-    </row>
-    <row r="734" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O734" s="1"/>
-      <c r="P734" s="1"/>
-    </row>
-    <row r="735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O735" s="1"/>
-      <c r="P735" s="1"/>
-    </row>
-    <row r="736" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O736" s="1"/>
-      <c r="P736" s="1"/>
-    </row>
-    <row r="737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O737" s="1"/>
-      <c r="P737" s="1"/>
-    </row>
-    <row r="738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O738" s="1"/>
-      <c r="P738" s="1"/>
-    </row>
-    <row r="739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O739" s="1"/>
-      <c r="P739" s="1"/>
-    </row>
-    <row r="740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O740" s="1"/>
-      <c r="P740" s="1"/>
-    </row>
-    <row r="741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O741" s="1"/>
-      <c r="P741" s="1"/>
-    </row>
-    <row r="742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O742" s="1"/>
-      <c r="P742" s="1"/>
-    </row>
-    <row r="743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O743" s="1"/>
-      <c r="P743" s="1"/>
-    </row>
-    <row r="744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O744" s="1"/>
-      <c r="P744" s="1"/>
-    </row>
-    <row r="745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O745" s="1"/>
-      <c r="P745" s="1"/>
-    </row>
-    <row r="746" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O746" s="1"/>
-      <c r="P746" s="1"/>
-    </row>
-    <row r="747" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O747" s="1"/>
-      <c r="P747" s="1"/>
-    </row>
-    <row r="748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O748" s="1"/>
-      <c r="P748" s="1"/>
-    </row>
-    <row r="749" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O749" s="1"/>
-      <c r="P749" s="1"/>
-    </row>
-    <row r="750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O750" s="1"/>
-      <c r="P750" s="1"/>
-    </row>
-    <row r="751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O751" s="1"/>
-      <c r="P751" s="1"/>
-    </row>
-    <row r="752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O752" s="1"/>
-      <c r="P752" s="1"/>
-    </row>
-    <row r="753" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O753" s="1"/>
-      <c r="P753" s="1"/>
-    </row>
-    <row r="754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O754" s="1"/>
-      <c r="P754" s="1"/>
-    </row>
-    <row r="755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O755" s="1"/>
-      <c r="P755" s="1"/>
-    </row>
-    <row r="756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O756" s="1"/>
-      <c r="P756" s="1"/>
-    </row>
-    <row r="757" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O757" s="1"/>
-      <c r="P757" s="1"/>
-    </row>
-    <row r="758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O758" s="1"/>
-      <c r="P758" s="1"/>
-    </row>
-    <row r="759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O759" s="1"/>
-      <c r="P759" s="1"/>
-    </row>
-    <row r="760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O760" s="1"/>
-      <c r="P760" s="1"/>
-    </row>
-    <row r="761" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O761" s="1"/>
-      <c r="P761" s="1"/>
-    </row>
-    <row r="762" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O762" s="1"/>
-      <c r="P762" s="1"/>
-    </row>
-    <row r="763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O763" s="1"/>
-      <c r="P763" s="1"/>
-    </row>
-    <row r="764" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O764" s="1"/>
-      <c r="P764" s="1"/>
-    </row>
-    <row r="765" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O765" s="1"/>
-      <c r="P765" s="1"/>
-    </row>
-    <row r="766" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O766" s="1"/>
-      <c r="P766" s="1"/>
-    </row>
-    <row r="767" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O767" s="1"/>
-      <c r="P767" s="1"/>
-    </row>
-    <row r="768" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O768" s="1"/>
-      <c r="P768" s="1"/>
-    </row>
-    <row r="769" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O769" s="1"/>
-      <c r="P769" s="1"/>
-    </row>
-    <row r="770" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O770" s="1"/>
-      <c r="P770" s="1"/>
-    </row>
-    <row r="771" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O771" s="1"/>
-      <c r="P771" s="1"/>
-    </row>
-    <row r="772" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O772" s="1"/>
-      <c r="P772" s="1"/>
-    </row>
-    <row r="773" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O773" s="1"/>
-      <c r="P773" s="1"/>
-    </row>
-    <row r="774" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O774" s="1"/>
-      <c r="P774" s="1"/>
-    </row>
-    <row r="775" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O775" s="1"/>
-      <c r="P775" s="1"/>
-    </row>
-    <row r="776" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O776" s="1"/>
-      <c r="P776" s="1"/>
-    </row>
-    <row r="777" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O777" s="1"/>
-      <c r="P777" s="1"/>
-    </row>
-    <row r="778" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O778" s="1"/>
-      <c r="P778" s="1"/>
-    </row>
-    <row r="779" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O779" s="1"/>
-      <c r="P779" s="1"/>
-    </row>
-    <row r="780" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O780" s="1"/>
-      <c r="P780" s="1"/>
-    </row>
-    <row r="781" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O781" s="1"/>
-      <c r="P781" s="1"/>
-    </row>
-    <row r="782" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O782" s="1"/>
-      <c r="P782" s="1"/>
-    </row>
-    <row r="783" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O783" s="1"/>
-      <c r="P783" s="1"/>
-    </row>
-    <row r="784" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O784" s="1"/>
-      <c r="P784" s="1"/>
-    </row>
-    <row r="785" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O785" s="1"/>
-      <c r="P785" s="1"/>
-    </row>
-    <row r="786" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O786" s="1"/>
-      <c r="P786" s="1"/>
-    </row>
-    <row r="787" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O787" s="1"/>
-      <c r="P787" s="1"/>
-    </row>
-    <row r="788" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O788" s="1"/>
-      <c r="P788" s="1"/>
-    </row>
-    <row r="789" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O789" s="1"/>
-      <c r="P789" s="1"/>
-    </row>
-    <row r="790" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O790" s="1"/>
-      <c r="P790" s="1"/>
-    </row>
-    <row r="791" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O791" s="1"/>
-      <c r="P791" s="1"/>
-    </row>
-    <row r="792" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O792" s="1"/>
-      <c r="P792" s="1"/>
-    </row>
-    <row r="793" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O793" s="1"/>
-      <c r="P793" s="1"/>
-    </row>
-    <row r="794" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O794" s="1"/>
-      <c r="P794" s="1"/>
-    </row>
-    <row r="795" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O795" s="1"/>
-      <c r="P795" s="1"/>
-    </row>
-    <row r="796" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O796" s="1"/>
-      <c r="P796" s="1"/>
-    </row>
-    <row r="797" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O797" s="1"/>
-      <c r="P797" s="1"/>
-    </row>
-    <row r="798" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O798" s="1"/>
-      <c r="P798" s="1"/>
-    </row>
-    <row r="799" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O799" s="1"/>
-      <c r="P799" s="1"/>
-    </row>
-    <row r="800" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O800" s="1"/>
-      <c r="P800" s="1"/>
-    </row>
-    <row r="801" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O801" s="1"/>
-      <c r="P801" s="1"/>
-    </row>
-    <row r="802" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O802" s="1"/>
-      <c r="P802" s="1"/>
-    </row>
-    <row r="803" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O803" s="1"/>
-      <c r="P803" s="1"/>
-    </row>
-    <row r="804" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O804" s="1"/>
-      <c r="P804" s="1"/>
-    </row>
-    <row r="805" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O805" s="1"/>
-      <c r="P805" s="1"/>
-    </row>
-    <row r="806" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O806" s="1"/>
-      <c r="P806" s="1"/>
-    </row>
-    <row r="807" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O807" s="1"/>
-      <c r="P807" s="1"/>
-    </row>
-    <row r="808" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O808" s="1"/>
-      <c r="P808" s="1"/>
-    </row>
-    <row r="809" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O809" s="1"/>
-      <c r="P809" s="1"/>
-    </row>
-    <row r="810" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O810" s="1"/>
-      <c r="P810" s="1"/>
-    </row>
-    <row r="811" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O811" s="1"/>
-      <c r="P811" s="1"/>
-    </row>
-    <row r="812" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O812" s="1"/>
-      <c r="P812" s="1"/>
-    </row>
-    <row r="813" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O813" s="1"/>
-      <c r="P813" s="1"/>
-    </row>
-    <row r="814" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O814" s="1"/>
-      <c r="P814" s="1"/>
-    </row>
-    <row r="815" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O815" s="1"/>
-      <c r="P815" s="1"/>
-    </row>
-    <row r="816" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O816" s="1"/>
-      <c r="P816" s="1"/>
-    </row>
-    <row r="817" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O817" s="1"/>
-      <c r="P817" s="1"/>
-    </row>
-    <row r="818" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O818" s="1"/>
-      <c r="P818" s="1"/>
-    </row>
-    <row r="819" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O819" s="1"/>
-      <c r="P819" s="1"/>
-    </row>
-    <row r="820" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O820" s="1"/>
-      <c r="P820" s="1"/>
-    </row>
-    <row r="821" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O821" s="1"/>
-      <c r="P821" s="1"/>
-    </row>
-    <row r="822" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O822" s="1"/>
-      <c r="P822" s="1"/>
-    </row>
-    <row r="823" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O823" s="1"/>
-      <c r="P823" s="1"/>
-    </row>
-    <row r="824" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O824" s="1"/>
-      <c r="P824" s="1"/>
-    </row>
-    <row r="825" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O825" s="1"/>
-      <c r="P825" s="1"/>
-    </row>
-    <row r="826" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O826" s="1"/>
-      <c r="P826" s="1"/>
-    </row>
-    <row r="827" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O827" s="1"/>
-      <c r="P827" s="1"/>
-    </row>
-    <row r="828" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O828" s="1"/>
-      <c r="P828" s="1"/>
-    </row>
-    <row r="829" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O829" s="1"/>
-      <c r="P829" s="1"/>
-    </row>
-    <row r="830" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O830" s="1"/>
-      <c r="P830" s="1"/>
-    </row>
-    <row r="831" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O831" s="1"/>
-      <c r="P831" s="1"/>
-    </row>
-    <row r="832" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O832" s="1"/>
-      <c r="P832" s="1"/>
-    </row>
-    <row r="833" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O833" s="1"/>
-      <c r="P833" s="1"/>
-    </row>
-    <row r="834" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O834" s="1"/>
-      <c r="P834" s="1"/>
-    </row>
-    <row r="835" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O835" s="1"/>
-      <c r="P835" s="1"/>
-    </row>
-    <row r="836" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O836" s="1"/>
-      <c r="P836" s="1"/>
-    </row>
-    <row r="837" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O837" s="1"/>
-      <c r="P837" s="1"/>
-    </row>
-    <row r="838" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O838" s="1"/>
-      <c r="P838" s="1"/>
-    </row>
-    <row r="839" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O839" s="1"/>
-      <c r="P839" s="1"/>
-    </row>
-    <row r="840" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O840" s="1"/>
-      <c r="P840" s="1"/>
-    </row>
-    <row r="841" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O841" s="1"/>
-      <c r="P841" s="1"/>
-    </row>
-    <row r="842" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O842" s="1"/>
-      <c r="P842" s="1"/>
-    </row>
-    <row r="843" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O843" s="1"/>
-      <c r="P843" s="1"/>
-    </row>
-    <row r="844" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O844" s="1"/>
-      <c r="P844" s="1"/>
-    </row>
-    <row r="845" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O845" s="1"/>
-      <c r="P845" s="1"/>
-    </row>
-    <row r="846" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O846" s="1"/>
-      <c r="P846" s="1"/>
-    </row>
-    <row r="847" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O847" s="1"/>
-      <c r="P847" s="1"/>
-    </row>
-    <row r="848" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O848" s="1"/>
-      <c r="P848" s="1"/>
-    </row>
-    <row r="849" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O849" s="1"/>
-      <c r="P849" s="1"/>
-    </row>
-    <row r="850" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O850" s="1"/>
-      <c r="P850" s="1"/>
-    </row>
-    <row r="851" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O851" s="1"/>
-      <c r="P851" s="1"/>
-    </row>
-    <row r="852" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O852" s="1"/>
-      <c r="P852" s="1"/>
-    </row>
-    <row r="853" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O853" s="1"/>
-      <c r="P853" s="1"/>
-    </row>
-    <row r="854" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O854" s="1"/>
-      <c r="P854" s="1"/>
-    </row>
-    <row r="855" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O855" s="1"/>
-      <c r="P855" s="1"/>
-    </row>
-    <row r="856" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O856" s="1"/>
-      <c r="P856" s="1"/>
-    </row>
-    <row r="857" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O857" s="1"/>
-      <c r="P857" s="1"/>
-    </row>
-    <row r="858" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O858" s="1"/>
-      <c r="P858" s="1"/>
-    </row>
-    <row r="859" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O859" s="1"/>
-      <c r="P859" s="1"/>
-    </row>
-    <row r="860" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O860" s="1"/>
-      <c r="P860" s="1"/>
-    </row>
-    <row r="861" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O861" s="1"/>
-      <c r="P861" s="1"/>
-    </row>
-    <row r="862" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O862" s="1"/>
-      <c r="P862" s="1"/>
-    </row>
-    <row r="863" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O863" s="1"/>
-      <c r="P863" s="1"/>
-    </row>
-    <row r="864" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O864" s="1"/>
-      <c r="P864" s="1"/>
-    </row>
-    <row r="865" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O865" s="1"/>
-      <c r="P865" s="1"/>
-    </row>
-    <row r="866" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O866" s="1"/>
-      <c r="P866" s="1"/>
-    </row>
-    <row r="867" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O867" s="1"/>
-      <c r="P867" s="1"/>
-    </row>
-    <row r="868" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O868" s="1"/>
-      <c r="P868" s="1"/>
-    </row>
-    <row r="869" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O869" s="1"/>
-      <c r="P869" s="1"/>
-    </row>
-    <row r="870" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O870" s="1"/>
-      <c r="P870" s="1"/>
-    </row>
-    <row r="871" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O871" s="1"/>
-      <c r="P871" s="1"/>
-    </row>
-    <row r="872" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O872" s="1"/>
-      <c r="P872" s="1"/>
-    </row>
-    <row r="873" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O873" s="1"/>
-      <c r="P873" s="1"/>
-    </row>
-    <row r="874" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O874" s="1"/>
-      <c r="P874" s="1"/>
-    </row>
-    <row r="875" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O875" s="1"/>
-      <c r="P875" s="1"/>
-    </row>
-    <row r="876" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O876" s="1"/>
-      <c r="P876" s="1"/>
-    </row>
-    <row r="877" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O877" s="1"/>
-      <c r="P877" s="1"/>
-    </row>
-    <row r="878" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O878" s="1"/>
-      <c r="P878" s="1"/>
-    </row>
-    <row r="879" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O879" s="1"/>
-      <c r="P879" s="1"/>
-    </row>
-    <row r="880" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O880" s="1"/>
-      <c r="P880" s="1"/>
-    </row>
-    <row r="881" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O881" s="1"/>
-      <c r="P881" s="1"/>
-    </row>
-    <row r="882" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O882" s="1"/>
-      <c r="P882" s="1"/>
-    </row>
-    <row r="883" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O883" s="1"/>
-      <c r="P883" s="1"/>
-    </row>
-    <row r="884" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O884" s="1"/>
-      <c r="P884" s="1"/>
-    </row>
-    <row r="885" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O885" s="1"/>
-      <c r="P885" s="1"/>
-    </row>
-    <row r="886" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O886" s="1"/>
-      <c r="P886" s="1"/>
-    </row>
-    <row r="887" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O887" s="1"/>
-      <c r="P887" s="1"/>
-    </row>
-    <row r="888" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O888" s="1"/>
-      <c r="P888" s="1"/>
-    </row>
-    <row r="889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O889" s="1"/>
-      <c r="P889" s="1"/>
-    </row>
-    <row r="890" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O890" s="1"/>
-      <c r="P890" s="1"/>
-    </row>
-    <row r="891" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O891" s="1"/>
-      <c r="P891" s="1"/>
-    </row>
-    <row r="892" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O892" s="1"/>
-      <c r="P892" s="1"/>
-    </row>
-    <row r="893" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O893" s="1"/>
-      <c r="P893" s="1"/>
-    </row>
-    <row r="894" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O894" s="1"/>
-      <c r="P894" s="1"/>
-    </row>
-    <row r="895" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O895" s="1"/>
-      <c r="P895" s="1"/>
-    </row>
-    <row r="896" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O896" s="1"/>
-      <c r="P896" s="1"/>
-    </row>
-    <row r="897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O897" s="1"/>
-      <c r="P897" s="1"/>
-    </row>
-    <row r="898" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O898" s="1"/>
-      <c r="P898" s="1"/>
-    </row>
-    <row r="899" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O899" s="1"/>
-      <c r="P899" s="1"/>
-    </row>
-    <row r="900" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O900" s="1"/>
-      <c r="P900" s="1"/>
-    </row>
-    <row r="901" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O901" s="1"/>
-      <c r="P901" s="1"/>
-    </row>
-    <row r="902" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O902" s="1"/>
-      <c r="P902" s="1"/>
-    </row>
-    <row r="903" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O903" s="1"/>
-      <c r="P903" s="1"/>
-    </row>
-    <row r="904" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O904" s="1"/>
-      <c r="P904" s="1"/>
-    </row>
-    <row r="905" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O905" s="1"/>
-      <c r="P905" s="1"/>
-    </row>
-    <row r="906" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O906" s="1"/>
-      <c r="P906" s="1"/>
-    </row>
-    <row r="907" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O907" s="1"/>
-      <c r="P907" s="1"/>
-    </row>
-    <row r="908" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O908" s="1"/>
-      <c r="P908" s="1"/>
-    </row>
-    <row r="909" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O909" s="1"/>
-      <c r="P909" s="1"/>
-    </row>
-    <row r="910" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O910" s="1"/>
-      <c r="P910" s="1"/>
-    </row>
-    <row r="911" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O911" s="1"/>
-      <c r="P911" s="1"/>
-    </row>
-    <row r="912" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O912" s="1"/>
-      <c r="P912" s="1"/>
-    </row>
-    <row r="913" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O913" s="1"/>
-      <c r="P913" s="1"/>
-    </row>
-    <row r="914" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O914" s="1"/>
-      <c r="P914" s="1"/>
-    </row>
-    <row r="915" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O915" s="1"/>
-      <c r="P915" s="1"/>
-    </row>
-    <row r="916" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O916" s="1"/>
-      <c r="P916" s="1"/>
-    </row>
-    <row r="917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O917" s="1"/>
-      <c r="P917" s="1"/>
-    </row>
-    <row r="918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O918" s="1"/>
-      <c r="P918" s="1"/>
-    </row>
-    <row r="919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O919" s="1"/>
-      <c r="P919" s="1"/>
-    </row>
-    <row r="920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O920" s="1"/>
-      <c r="P920" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -9117,7 +5591,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.11"/>
   </cols>
@@ -25556,7 +22030,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.29"/>
@@ -25769,7 +22243,7 @@
       <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -26289,7 +22763,7 @@
       <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
plotted 2019 protein and cn ratios
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="2017-fluxes" sheetId="1" state="visible" r:id="rId2"/>
@@ -1063,7 +1063,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart87.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart111.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1249,11 +1249,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="49318673"/>
-        <c:axId val="86099962"/>
+        <c:axId val="24192654"/>
+        <c:axId val="85248195"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49318673"/>
+        <c:axId val="24192654"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,12 +1309,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86099962"/>
+        <c:crossAx val="85248195"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86099962"/>
+        <c:axId val="85248195"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1379,7 +1379,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49318673"/>
+        <c:crossAx val="24192654"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1427,7 +1427,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart88.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart112.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1625,11 +1625,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="28099833"/>
-        <c:axId val="48082877"/>
+        <c:axId val="71001927"/>
+        <c:axId val="76358127"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="28099833"/>
+        <c:axId val="71001927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,12 +1685,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48082877"/>
+        <c:crossAx val="76358127"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48082877"/>
+        <c:axId val="76358127"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1755,7 +1755,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28099833"/>
+        <c:crossAx val="71001927"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1803,7 +1803,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart89.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart113.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1989,11 +1989,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="30403148"/>
-        <c:axId val="29242847"/>
+        <c:axId val="2120184"/>
+        <c:axId val="31424293"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30403148"/>
+        <c:axId val="2120184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2049,12 +2049,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29242847"/>
+        <c:crossAx val="31424293"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29242847"/>
+        <c:axId val="31424293"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2119,7 +2119,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30403148"/>
+        <c:crossAx val="2120184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2167,7 +2167,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart90.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart114.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2365,11 +2365,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99514331"/>
-        <c:axId val="85036926"/>
+        <c:axId val="67512238"/>
+        <c:axId val="57275574"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99514331"/>
+        <c:axId val="67512238"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2425,12 +2425,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85036926"/>
+        <c:crossAx val="57275574"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85036926"/>
+        <c:axId val="57275574"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2495,7 +2495,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99514331"/>
+        <c:crossAx val="67512238"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2543,7 +2543,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart91.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart115.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2776,11 +2776,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="25628793"/>
-        <c:axId val="51226124"/>
+        <c:axId val="15346504"/>
+        <c:axId val="29059702"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="25628793"/>
+        <c:axId val="15346504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2808,12 +2808,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51226124"/>
+        <c:crossAx val="29059702"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51226124"/>
+        <c:axId val="29059702"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2850,7 +2850,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25628793"/>
+        <c:crossAx val="15346504"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2877,7 +2877,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart92.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart116.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3185,11 +3185,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="45919150"/>
-        <c:axId val="52012145"/>
+        <c:axId val="92195234"/>
+        <c:axId val="27811602"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45919150"/>
+        <c:axId val="92195234"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3217,12 +3217,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52012145"/>
+        <c:crossAx val="27811602"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52012145"/>
+        <c:axId val="27811602"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3259,7 +3259,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45919150"/>
+        <c:crossAx val="92195234"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3492,8 +3492,8 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3934,9 +3934,6 @@
       <c r="I14" s="1" t="n">
         <v>169.7946237</v>
       </c>
-      <c r="J14" s="1" t="n">
-        <v>1286.93766937669</v>
-      </c>
       <c r="K14" s="1" t="n">
         <v>1286.93766937669</v>
       </c>
@@ -4125,9 +4122,6 @@
       </c>
       <c r="I20" s="1" t="n">
         <v>39.43923292</v>
-      </c>
-      <c r="J20" s="1" t="n">
-        <v>1225.07678410117</v>
       </c>
       <c r="K20" s="1" t="n">
         <v>1225.07678410117</v>
@@ -22759,540 +22753,543 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.63"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>314.713043550195</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>314.713043550195</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <f aca="false">D6/$D$6</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>119</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>119</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>120</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>120</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>120</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>120</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>314.713043550195</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>314.713043550195</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <f aca="false">D18/$D$6</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>140</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>148</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>1920.24529660616</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>1920.24529660616</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <f aca="false">D21/$D$6</f>
         <v>6.10157518399739</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>159</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>159</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>179</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>179</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="1" t="n">
         <v>510.117646938796</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>510.117646938796</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="1" t="n">
         <f aca="false">D31/$D$6</f>
         <v>1.62089769519653</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="C32" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="1" t="n">
         <v>224.640400250156</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>224.640400250156</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32" s="1" t="n">
         <f aca="false">D32/$D$6</f>
         <v>0.713794375079109</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="C33" s="1" t="n">
         <v>265</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34" s="1" t="n">
         <v>312</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C35" s="1" t="n">
         <v>312</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="1" t="n">
         <v>365</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="1" t="n">
         <v>43.3505226579923</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>43.3505226579923</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F36" s="1" t="n">
         <f aca="false">D36/$D$6</f>
         <v>0.137746189890849</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37" s="1" t="n">
         <v>365</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C38" s="1" t="n">
         <v>412</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39" s="1" t="n">
         <v>452</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="C40" s="1" t="n">
         <v>452</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41" s="1" t="n">
         <v>965</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42" s="1" t="n">
         <v>965</v>
       </c>
     </row>

</xml_diff>

<commit_message>
calc b after 120 150 for p2 p1 2017 protein flux
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2017-fluxes" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="278">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -856,16 +856,23 @@
   </si>
   <si>
     <t xml:space="preserve">Normalized to F100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normalized to 120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normalized to F150</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -1047,7 +1054,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004586"/>
@@ -1063,7 +1070,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart111.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart156.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1249,11 +1256,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="24192654"/>
-        <c:axId val="85248195"/>
+        <c:axId val="23404603"/>
+        <c:axId val="33537181"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="24192654"/>
+        <c:axId val="23404603"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,12 +1316,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85248195"/>
+        <c:crossAx val="33537181"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85248195"/>
+        <c:axId val="33537181"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1379,7 +1386,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24192654"/>
+        <c:crossAx val="23404603"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1427,7 +1434,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart112.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart157.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1625,11 +1632,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="71001927"/>
-        <c:axId val="76358127"/>
+        <c:axId val="47167144"/>
+        <c:axId val="76166948"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71001927"/>
+        <c:axId val="47167144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,12 +1692,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76358127"/>
+        <c:crossAx val="76166948"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76358127"/>
+        <c:axId val="76166948"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1755,7 +1762,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71001927"/>
+        <c:crossAx val="47167144"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1803,7 +1810,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart113.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart158.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1989,11 +1996,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="2120184"/>
-        <c:axId val="31424293"/>
+        <c:axId val="72770093"/>
+        <c:axId val="94146951"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2120184"/>
+        <c:axId val="72770093"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2049,12 +2056,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31424293"/>
+        <c:crossAx val="94146951"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="31424293"/>
+        <c:axId val="94146951"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2119,7 +2126,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2120184"/>
+        <c:crossAx val="72770093"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2167,7 +2174,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart114.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart159.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2365,11 +2372,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="67512238"/>
-        <c:axId val="57275574"/>
+        <c:axId val="94601459"/>
+        <c:axId val="68854850"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67512238"/>
+        <c:axId val="94601459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2425,12 +2432,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57275574"/>
+        <c:crossAx val="68854850"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57275574"/>
+        <c:axId val="68854850"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2495,7 +2502,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67512238"/>
+        <c:crossAx val="94601459"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2543,12 +2550,40 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart115.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart160.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>B. Coastal P1 2017</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2569,18 +2604,18 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="579d1c"/>
+              <a:srgbClr val="004586"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
+            <c:symbol val="square"/>
             <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c"/>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -2626,67 +2661,165 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'protein power function P1'!$D$2:$D$29</c:f>
+              <c:f>'protein power function P1'!$G$18:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>329.466918726015</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0525615721397825</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.483030699662425</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>255.065217455071</c:v>
+                  <c:v>0.396291345363287</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1786.95652173913</c:v>
+                <c:pt idx="7">
+                  <c:v>0.189735985361204</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>240.000000011294</c:v>
+                <c:pt idx="8">
+                  <c:v>0.172702308459285</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>952.869565217391</c:v>
+                <c:pt idx="9">
+                  <c:v>0.369366656629528</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>303.109565120396</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>277.874396135266</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>340.043478260869</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3484.17391304348</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>183.133658477983</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1682.96296296296</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1380.74796747967</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>661.073170561108</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>601.724877856229</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1286.93766937669</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>46.3317073217063</c:v>
+                <c:pt idx="10">
+                  <c:v>0.0132977596635625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'protein power function P1'!$C$2:$C$29</c:f>
+              <c:f>'protein power function P1'!$C$18:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'protein power function P1'!$G$2:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.0945609854584499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0732067984609493</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.51287810721773</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0688828990748198</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.273485075371868</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0869961065909093</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0797533082648387</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0975965858041328</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'protein power function P1'!$C$2:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -2735,57 +2868,49 @@
                 <c:pt idx="15">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>168</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>355</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>355</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>700</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="15346504"/>
-        <c:axId val="29059702"/>
+        <c:axId val="58138505"/>
+        <c:axId val="62344689"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="15346504"/>
+        <c:axId val="58138505"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Protein flux normalized to 120 m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -2808,26 +2933,45 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29059702"/>
+        <c:crossAx val="62344689"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29059702"/>
+        <c:axId val="62344689"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
-        </c:majorGridlines>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -2850,7 +2994,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15346504"/>
+        <c:crossAx val="58138505"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2877,12 +3021,40 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart116.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart161.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>A. Offhore P2 2017</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2930,42 +3102,9 @@
               </c:spPr>
             </c:marker>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="29"/>
-            <c:marker>
-              <c:symbol val="square"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="29"/>
               <c:txPr>
                 <a:bodyPr wrap="none"/>
                 <a:lstStyle/>
@@ -3026,175 +3165,232 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'protein power function P2'!$F$2:$F$42</c:f>
+              <c:f>'protein power function P2'!$F$21:$F$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
-                <c:pt idx="4">
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
+                <c:pt idx="10">
+                  <c:v>0.265652335063847</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>6.10157518399739</c:v>
+                <c:pt idx="11">
+                  <c:v>0.116985262584517</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.62089769519653</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.713794375079109</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.137746189890849</c:v>
+                <c:pt idx="15">
+                  <c:v>0.0225755130006619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'protein power function P2'!$C$2:$C$42</c:f>
+              <c:f>'protein power function P2'!$C$21:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>59</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>113</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>113</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>119</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>119</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>120</c:v>
+                  <c:v>312</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>120</c:v>
+                  <c:v>312</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>159</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>159</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>179</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>179</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>265</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>312</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>312</c:v>
-                </c:pt>
-                <c:pt idx="34">
                   <c:v>365</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>365</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>412</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>452</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>452</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>965</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="92195234"/>
-        <c:axId val="27811602"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'protein power function P2'!$F$6:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.163892104881818</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.163892104881818</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'protein power function P2'!$C$6:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="80057304"/>
+        <c:axId val="1983548"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92195234"/>
+        <c:axId val="80057304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Protein flux normalized to 150 m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -3217,26 +3413,45 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27811602"/>
+        <c:crossAx val="1983548"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="27811602"/>
+        <c:axId val="1983548"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
-        </c:majorGridlines>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -3259,7 +3474,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92195234"/>
+        <c:crossAx val="80057304"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3419,16 +3634,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>713880</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>781200</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>47880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>503280</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>471240</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>149400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3436,8 +3651,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5636160" y="210240"/>
-        <a:ext cx="4712040" cy="4406400"/>
+        <a:off x="6523920" y="535320"/>
+        <a:ext cx="2971800" cy="3840480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3454,16 +3669,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>694080</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>10080</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>761040</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>524520</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3471,8 +3686,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5616360" y="458640"/>
-        <a:ext cx="5810040" cy="3239640"/>
+        <a:off x="6187320" y="564480"/>
+        <a:ext cx="2975400" cy="4064040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -22231,505 +22446,575 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.63"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>329.466918726015</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>329.466918726015</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <f aca="false">D2/$D$13</f>
         <v>1.37277882796046</v>
       </c>
+      <c r="G2" s="1" t="n">
+        <f aca="false">D2/$D$18</f>
+        <v>0.0945609854584499</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>255.065217455071</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>255.065217455071</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <f aca="false">D5/$D$13</f>
         <v>1.06277173934612</v>
       </c>
+      <c r="G5" s="1" t="n">
+        <f aca="false">D5/$D$18</f>
+        <v>0.0732067984609493</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>1786.95652173913</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>1786.95652173913</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <f aca="false">D6/$D$13</f>
         <v>7.44565217356266</v>
       </c>
+      <c r="G6" s="1" t="n">
+        <f aca="false">D6/$D$18</f>
+        <v>0.51287810721773</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>240.000000011294</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>240.000000011294</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <f aca="false">D13/$D$13</f>
         <v>1</v>
       </c>
+      <c r="G13" s="1" t="n">
+        <f aca="false">D13/$D$18</f>
+        <v>0.0688828990748198</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>952.869565217391</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>952.869565217391</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <f aca="false">D14/$D$13</f>
         <v>3.97028985488563</v>
       </c>
+      <c r="G14" s="1" t="n">
+        <f aca="false">D14/$D$18</f>
+        <v>0.273485075371868</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>303.109565120396</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>303.109565120396</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <f aca="false">D15/$D$13</f>
         <v>1.26295652127555</v>
       </c>
+      <c r="G15" s="1" t="n">
+        <f aca="false">D15/$D$18</f>
+        <v>0.0869961065909093</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>277.874396135266</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>277.874396135266</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <f aca="false">D16/$D$13</f>
         <v>1.15780998384246</v>
       </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">D16/$D$18</f>
+        <v>0.0797533082648387</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>340.043478260869</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>340.043478260869</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <f aca="false">D17/$D$13</f>
         <v>1.41684782602028</v>
       </c>
+      <c r="G17" s="1" t="n">
+        <f aca="false">D17/$D$18</f>
+        <v>0.0975965858041328</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>3484.17391304348</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>3484.17391304348</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <f aca="false">D18/$D$13</f>
         <v>14.5173913036647</v>
       </c>
+      <c r="G18" s="1" t="n">
+        <f aca="false">D18/$D$18</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>183.133658477983</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>183.133658477983</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <f aca="false">D19/$D$13</f>
         <v>0.763056910289021</v>
       </c>
+      <c r="G19" s="1" t="n">
+        <f aca="false">D19/$D$18</f>
+        <v>0.0525615721397825</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>1682.96296296296</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>1682.96296296296</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <f aca="false">D20/$D$13</f>
         <v>7.01234567868235</v>
       </c>
+      <c r="G20" s="1" t="n">
+        <f aca="false">D20/$D$18</f>
+        <v>0.483030699662425</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>1380.74796747967</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>1380.74796747967</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <f aca="false">D21/$D$13</f>
         <v>5.75311653089456</v>
       </c>
+      <c r="G21" s="1" t="n">
+        <f aca="false">D21/$D$18</f>
+        <v>0.396291345363287</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>168</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>661.073170561108</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>661.073170561108</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="1" t="n">
         <f aca="false">D25/$D$13</f>
         <v>2.754471543875</v>
       </c>
+      <c r="G25" s="1" t="n">
+        <f aca="false">D25/$D$18</f>
+        <v>0.189735985361204</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>355</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>601.724877856229</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>601.724877856229</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="1" t="n">
         <f aca="false">D26/$D$13</f>
         <v>2.50718699094964</v>
       </c>
+      <c r="G26" s="1" t="n">
+        <f aca="false">D26/$D$18</f>
+        <v>0.172702308459285</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>355</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>1286.93766937669</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>1286.93766937669</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="1" t="n">
         <f aca="false">D27/$D$13</f>
         <v>5.3622402888172</v>
       </c>
+      <c r="G27" s="1" t="n">
+        <f aca="false">D27/$D$18</f>
+        <v>0.369366656629528</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>700</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>46.3317073217063</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>46.3317073217063</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="1" t="n">
         <f aca="false">D28/$D$13</f>
         <v>0.193048780498025</v>
       </c>
+      <c r="G28" s="1" t="n">
+        <f aca="false">D28/$D$18</f>
+        <v>0.0132977596635625</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>700</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>1225.07678410117</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="1" t="n">
         <f aca="false">D29/$D$13</f>
         <v>0</v>
       </c>
@@ -22753,13 +23038,14 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="11.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22779,7 +23065,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22843,8 +23129,8 @@
         <v>314.713043550195</v>
       </c>
       <c r="F6" s="1" t="n">
-        <f aca="false">D6/$D$6</f>
-        <v>1</v>
+        <f aca="false">D6/$D$21</f>
+        <v>0.163892104881818</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22985,8 +23271,8 @@
         <v>314.713043550195</v>
       </c>
       <c r="F18" s="1" t="n">
-        <f aca="false">D18/$D$6</f>
-        <v>1</v>
+        <f aca="false">D18/$D$21</f>
+        <v>0.163892104881818</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23028,8 +23314,8 @@
         <v>1920.24529660616</v>
       </c>
       <c r="F21" s="1" t="n">
-        <f aca="false">D21/$D$6</f>
-        <v>6.10157518399739</v>
+        <f aca="false">D21/$D$21</f>
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23148,8 +23434,8 @@
         <v>510.117646938796</v>
       </c>
       <c r="F31" s="1" t="n">
-        <f aca="false">D31/$D$6</f>
-        <v>1.62089769519653</v>
+        <f aca="false">D31/$D$21</f>
+        <v>0.265652335063847</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23169,8 +23455,8 @@
         <v>224.640400250156</v>
       </c>
       <c r="F32" s="1" t="n">
-        <f aca="false">D32/$D$6</f>
-        <v>0.713794375079109</v>
+        <f aca="false">D32/$D$21</f>
+        <v>0.116985262584517</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23223,8 +23509,8 @@
         <v>43.3505226579923</v>
       </c>
       <c r="F36" s="1" t="n">
-        <f aca="false">D36/$D$6</f>
-        <v>0.137746189890849</v>
+        <f aca="false">D36/$D$21</f>
+        <v>0.0225755130006619</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
calc b values for protein flux attenuation
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="2017-fluxes" sheetId="1" state="visible" r:id="rId2"/>
@@ -1070,7 +1070,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart156.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart208.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1256,11 +1256,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="23404603"/>
-        <c:axId val="33537181"/>
+        <c:axId val="2542640"/>
+        <c:axId val="43301140"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="23404603"/>
+        <c:axId val="2542640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1316,12 +1316,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33537181"/>
+        <c:crossAx val="43301140"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33537181"/>
+        <c:axId val="43301140"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1386,7 +1386,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23404603"/>
+        <c:crossAx val="2542640"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1434,7 +1434,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart157.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart209.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1632,11 +1632,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="47167144"/>
-        <c:axId val="76166948"/>
+        <c:axId val="15058345"/>
+        <c:axId val="7297781"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47167144"/>
+        <c:axId val="15058345"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1692,12 +1692,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76166948"/>
+        <c:crossAx val="7297781"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76166948"/>
+        <c:axId val="7297781"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1762,7 +1762,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47167144"/>
+        <c:crossAx val="15058345"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1810,7 +1810,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart158.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart210.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1996,11 +1996,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="72770093"/>
-        <c:axId val="94146951"/>
+        <c:axId val="83511020"/>
+        <c:axId val="97075791"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72770093"/>
+        <c:axId val="83511020"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2056,12 +2056,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94146951"/>
+        <c:crossAx val="97075791"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94146951"/>
+        <c:axId val="97075791"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2126,7 +2126,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72770093"/>
+        <c:crossAx val="83511020"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2174,7 +2174,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart159.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart211.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2372,11 +2372,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="94601459"/>
-        <c:axId val="68854850"/>
+        <c:axId val="39617030"/>
+        <c:axId val="84029798"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94601459"/>
+        <c:axId val="39617030"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2432,12 +2432,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68854850"/>
+        <c:crossAx val="84029798"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68854850"/>
+        <c:axId val="84029798"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2502,7 +2502,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94601459"/>
+        <c:crossAx val="39617030"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2550,7 +2550,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart160.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart212.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2683,9 +2683,6 @@
                 <c:pt idx="8">
                   <c:v>0.172702308459285</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.369366656629528</c:v>
-                </c:pt>
                 <c:pt idx="10">
                   <c:v>0.0132977596635625</c:v>
                 </c:pt>
@@ -2873,11 +2870,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="58138505"/>
-        <c:axId val="62344689"/>
+        <c:axId val="46794556"/>
+        <c:axId val="79858805"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58138505"/>
+        <c:axId val="46794556"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2933,12 +2930,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62344689"/>
+        <c:crossAx val="79858805"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62344689"/>
+        <c:axId val="79858805"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2994,7 +2991,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58138505"/>
+        <c:crossAx val="46794556"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3021,7 +3018,866 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart161.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart213.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>B. Coastal P1 2017</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'protein power function P1'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normalized to F100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="579d1c"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'protein power function P1'!$G$2:$G$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0.0945609854584499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0732067984609493</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.51287810721773</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0688828990748198</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.273485075371868</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0869961065909093</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0797533082648387</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0975965858041328</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0525615721397825</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.483030699662425</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.396291345363287</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.189735985361204</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.172702308459285</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0132977596635625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'protein power function P1'!$C$2:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="67650518"/>
+        <c:axId val="71345861"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="67650518"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Protein flux normalized to 120 m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="71345861"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="71345861"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67650518"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart214.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>B. Coastal P1 2017</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'protein power function P1'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normalized to F100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="24"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="579d1c"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'protein power function P1'!$F$2:$F$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>1.37277882796046</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.06277173934612</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.44565217356266</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.97028985488563</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.26295652127555</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.15780998384246</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.41684782602028</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.5173913036647</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.763056910289021</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.01234567868235</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.75311653089456</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.754471543875</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.50718699094964</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.193048780498025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'protein power function P1'!$C$2:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="52286174"/>
+        <c:axId val="39858623"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="52286174"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Protein flux normalized to 100 m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="39858623"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="39858623"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="52286174"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart215.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3353,11 +4209,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="80057304"/>
-        <c:axId val="1983548"/>
+        <c:axId val="88523043"/>
+        <c:axId val="36155146"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80057304"/>
+        <c:axId val="88523043"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3413,12 +4269,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1983548"/>
+        <c:crossAx val="36155146"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1983548"/>
+        <c:axId val="36155146"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3474,8 +4330,941 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80057304"/>
+        <c:crossAx val="88523043"/>
         <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart216.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>A. Offhore P2 2017</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'protein power function P2'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Protein flux (ug/m2/day)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'protein power function P2'!$F$21:$F$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.265652335063847</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.116985262584517</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0225755130006619</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'protein power function P2'!$C$21:$C$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>365</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'protein power function P2'!$F$6:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.163892104881818</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.163892104881818</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'protein power function P2'!$C$6:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="69077197"/>
+        <c:axId val="21352036"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="69077197"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Protein flux normalized to 150 m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="21352036"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="21352036"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69077197"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart217.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>B. Coastal P1 2017</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'protein power function P1'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normalized to F100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="24"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="579d1c"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'protein power function P1'!$F$2:$F$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>1.37277882796046</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.06277173934612</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.44565217356266</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.97028985488563</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.26295652127555</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.15780998384246</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.41684782602028</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.5173913036647</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.763056910289021</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.01234567868235</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.75311653089456</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.754471543875</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.50718699094964</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.193048780498025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'protein power function P1'!$C$2:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="51077372"/>
+        <c:axId val="55734032"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="51077372"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Protein flux normalized to 100 m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="55734032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="55734032"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="51077372"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3599,16 +5388,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>294120</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>797400</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>689040</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>91080</xdr:rowOff>
+      <xdr:colOff>363600</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3616,7 +5405,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10514880" y="5192280"/>
+        <a:off x="10189440" y="5354640"/>
         <a:ext cx="5366880" cy="4814640"/>
       </xdr:xfrm>
       <a:graphic>
@@ -3662,6 +5451,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>632880</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>322920</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>120600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="9657360" y="506520"/>
+        <a:ext cx="2971800" cy="3840480"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>465120</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>153360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>155520</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>92520</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="12771360" y="478440"/>
+        <a:ext cx="2971800" cy="3840480"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3682,7 +5531,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvPr id="7" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3692,6 +5541,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>30240</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>48600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>540720</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133560</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="9488880" y="536040"/>
+        <a:ext cx="2971800" cy="3986640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>534960</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>48600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>225000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133560</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="12454920" y="536040"/>
+        <a:ext cx="2971800" cy="3986640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -22235,7 +24144,7 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -22448,8 +24357,8 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T25" activeCellId="0" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22961,20 +24870,6 @@
       <c r="C27" s="1" t="n">
         <v>355</v>
       </c>
-      <c r="D27" s="1" t="n">
-        <v>1286.93766937669</v>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>1286.93766937669</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <f aca="false">D27/$D$13</f>
-        <v>5.3622402888172</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <f aca="false">D27/$D$18</f>
-        <v>0.369366656629528</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
@@ -23013,10 +24908,6 @@
       </c>
       <c r="E29" s="1" t="n">
         <v>1225.07678410117</v>
-      </c>
-      <c r="F29" s="1" t="n">
-        <f aca="false">D29/$D$13</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -23038,8 +24929,8 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T27" activeCellId="0" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
made shitty composite figure from trap filter photos
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="289">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -862,6 +862,102 @@
   </si>
   <si>
     <t xml:space="preserve">Normalized to F150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normalized to 100 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change from surface to upper oxycline</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Table 4.2 Attenuation coefficients (</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) of bulk sinking particles and and protein in sinking particles</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sinking particle </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">b</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sinking particle protein </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">b</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Offshore P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coastal P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N. coastal P3</t>
   </si>
 </sst>
 </file>
@@ -874,7 +970,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -918,6 +1014,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -927,12 +1043,26 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -961,7 +1091,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -996,6 +1126,42 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1070,7 +1236,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart208.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart228.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1256,11 +1422,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="2542640"/>
-        <c:axId val="43301140"/>
+        <c:axId val="99300975"/>
+        <c:axId val="93468710"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2542640"/>
+        <c:axId val="99300975"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1316,12 +1482,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43301140"/>
+        <c:crossAx val="93468710"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43301140"/>
+        <c:axId val="93468710"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1386,7 +1552,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2542640"/>
+        <c:crossAx val="99300975"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1434,7 +1600,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart209.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart229.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1632,11 +1798,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="15058345"/>
-        <c:axId val="7297781"/>
+        <c:axId val="94028460"/>
+        <c:axId val="41126334"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="15058345"/>
+        <c:axId val="94028460"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1692,12 +1858,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7297781"/>
+        <c:crossAx val="41126334"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="7297781"/>
+        <c:axId val="41126334"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1762,7 +1928,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15058345"/>
+        <c:crossAx val="94028460"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1810,7 +1976,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart210.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart230.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1996,11 +2162,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="83511020"/>
-        <c:axId val="97075791"/>
+        <c:axId val="74212794"/>
+        <c:axId val="57055423"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83511020"/>
+        <c:axId val="74212794"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2056,12 +2222,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97075791"/>
+        <c:crossAx val="57055423"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97075791"/>
+        <c:axId val="57055423"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2126,7 +2292,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83511020"/>
+        <c:crossAx val="74212794"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2174,7 +2340,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart211.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart231.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2372,11 +2538,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="39617030"/>
-        <c:axId val="84029798"/>
+        <c:axId val="35145807"/>
+        <c:axId val="19598916"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39617030"/>
+        <c:axId val="35145807"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2432,12 +2598,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84029798"/>
+        <c:crossAx val="19598916"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84029798"/>
+        <c:axId val="19598916"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2502,7 +2668,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39617030"/>
+        <c:crossAx val="35145807"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2550,7 +2716,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart212.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart232.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2870,11 +3036,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="46794556"/>
-        <c:axId val="79858805"/>
+        <c:axId val="71962018"/>
+        <c:axId val="23629084"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46794556"/>
+        <c:axId val="71962018"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2930,12 +3096,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79858805"/>
+        <c:crossAx val="23629084"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79858805"/>
+        <c:axId val="23629084"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2991,7 +3157,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46794556"/>
+        <c:crossAx val="71962018"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3018,7 +3184,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart213.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart233.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3276,11 +3442,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="67650518"/>
-        <c:axId val="71345861"/>
+        <c:axId val="13462669"/>
+        <c:axId val="98183002"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67650518"/>
+        <c:axId val="13462669"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3336,12 +3502,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71345861"/>
+        <c:crossAx val="98183002"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71345861"/>
+        <c:axId val="98183002"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3397,7 +3563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67650518"/>
+        <c:crossAx val="13462669"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3424,7 +3590,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart214.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart234.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3729,11 +3895,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="52286174"/>
-        <c:axId val="39858623"/>
+        <c:axId val="18074471"/>
+        <c:axId val="18657558"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52286174"/>
+        <c:axId val="18074471"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3789,12 +3955,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39858623"/>
+        <c:crossAx val="18657558"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="39858623"/>
+        <c:axId val="18657558"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3850,7 +4016,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52286174"/>
+        <c:crossAx val="18074471"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3877,7 +4043,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart215.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart235.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4209,11 +4375,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="88523043"/>
-        <c:axId val="36155146"/>
+        <c:axId val="90615126"/>
+        <c:axId val="52589404"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88523043"/>
+        <c:axId val="90615126"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4269,12 +4435,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36155146"/>
+        <c:crossAx val="52589404"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="36155146"/>
+        <c:axId val="52589404"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4330,7 +4496,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88523043"/>
+        <c:crossAx val="90615126"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4357,7 +4523,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart216.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart236.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4438,9 +4604,42 @@
               </c:spPr>
             </c:marker>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
               <c:txPr>
                 <a:bodyPr wrap="none"/>
                 <a:lstStyle/>
@@ -4501,77 +4700,125 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'protein power function P2'!$F$21:$F$36</c:f>
+              <c:f>'protein power function P2'!$G$6:$G$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.265652335063847</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.116985262584517</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0225755130006619</c:v>
+                  <c:v>6.10157518399739</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.62089769519653</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.713794375079109</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.137746189890849</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'protein power function P2'!$C$21:$C$36</c:f>
+              <c:f>'protein power function P2'!$C$6:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="16">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="17">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="18">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="19">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="20">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="21">
                   <c:v>159</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="22">
                   <c:v>159</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="23">
                   <c:v>179</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="24">
                   <c:v>179</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="25">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="26">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="27">
                   <c:v>265</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="28">
                   <c:v>312</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="29">
                   <c:v>312</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="30">
                   <c:v>365</c:v>
                 </c:pt>
               </c:numCache>
@@ -4579,121 +4826,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'protein power function P2'!$F$6:$F$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0.163892104881818</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.163892104881818</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'protein power function P2'!$C$6:$C$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>119</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>119</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>140</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="69077197"/>
-        <c:axId val="21352036"/>
+        <c:axId val="93553210"/>
+        <c:axId val="80038995"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69077197"/>
+        <c:axId val="93553210"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4714,7 +4851,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Protein flux normalized to 150 m</a:t>
+                  <a:t>Protein flux normalized to 100 m</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4749,12 +4886,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21352036"/>
+        <c:crossAx val="80038995"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21352036"/>
+        <c:axId val="80038995"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4810,7 +4947,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69077197"/>
+        <c:crossAx val="93553210"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4837,7 +4974,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart217.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart237.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5142,11 +5279,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="51077372"/>
-        <c:axId val="55734032"/>
+        <c:axId val="84466724"/>
+        <c:axId val="73648175"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51077372"/>
+        <c:axId val="84466724"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5202,12 +5339,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55734032"/>
+        <c:crossAx val="73648175"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55734032"/>
+        <c:axId val="73648175"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5263,7 +5400,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51077372"/>
+        <c:crossAx val="84466724"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5518,16 +5655,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>632880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>524520</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>614880</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5535,7 +5672,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6187320" y="564480"/>
+        <a:off x="11051280" y="488520"/>
         <a:ext cx="2975400" cy="4064040"/>
       </xdr:xfrm>
       <a:graphic>
@@ -5548,16 +5685,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>30240</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>622440</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>540720</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>312840</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5565,7 +5702,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9488880" y="536040"/>
+        <a:off x="14034240" y="450000"/>
         <a:ext cx="2971800" cy="3986640"/>
       </xdr:xfrm>
       <a:graphic>
@@ -5578,16 +5715,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>534960</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>307080</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>225000</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>817560</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5595,7 +5732,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12454920" y="536040"/>
+        <a:off x="17000280" y="450000"/>
         <a:ext cx="2971800" cy="3986640"/>
       </xdr:xfrm>
       <a:graphic>
@@ -24927,16 +25064,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T27" activeCellId="0" sqref="T27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="11.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="11.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24958,6 +25100,12 @@
       <c r="F1" s="1" t="s">
         <v>277</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -25023,6 +25171,10 @@
         <f aca="false">D6/$D$21</f>
         <v>0.163892104881818</v>
       </c>
+      <c r="G6" s="1" t="n">
+        <f aca="false">D6/$D$6</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -25208,6 +25360,10 @@
         <f aca="false">D21/$D$21</f>
         <v>1</v>
       </c>
+      <c r="G21" s="1" t="n">
+        <f aca="false">D21/$D$6</f>
+        <v>6.10157518399739</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -25328,6 +25484,10 @@
         <f aca="false">D31/$D$21</f>
         <v>0.265652335063847</v>
       </c>
+      <c r="G31" s="1" t="n">
+        <f aca="false">D31/$D$6</f>
+        <v>1.62089769519653</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
@@ -25349,6 +25509,10 @@
         <f aca="false">D32/$D$21</f>
         <v>0.116985262584517</v>
       </c>
+      <c r="G32" s="1" t="n">
+        <f aca="false">D32/$D$6</f>
+        <v>0.713794375079109</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -25360,6 +25524,9 @@
       <c r="C33" s="1" t="n">
         <v>265</v>
       </c>
+      <c r="I33" s="1" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
@@ -25372,7 +25539,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>81</v>
       </c>
@@ -25382,8 +25549,20 @@
       <c r="C35" s="1" t="n">
         <v>312</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I35" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>83</v>
       </c>
@@ -25403,8 +25582,25 @@
         <f aca="false">D36/$D$21</f>
         <v>0.0225755130006619</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="1" t="n">
+        <f aca="false">D36/$D$6</f>
+        <v>0.137746189890849</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="K36" s="12" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="L36" s="12" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="M36" s="13"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>84</v>
       </c>
@@ -25414,8 +25610,21 @@
       <c r="C37" s="1" t="n">
         <v>365</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I37" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="K37" s="12" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="L37" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="M37" s="13"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>82</v>
       </c>
@@ -25425,8 +25634,21 @@
       <c r="C38" s="1" t="n">
         <v>412</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I38" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="K38" s="12" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="L38" s="12" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="M38" s="13"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -25436,8 +25658,21 @@
       <c r="C39" s="1" t="n">
         <v>452</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I39" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="K39" s="12" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="L39" s="12" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="M39" s="13"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>86</v>
       </c>
@@ -25447,8 +25682,20 @@
       <c r="C40" s="1" t="n">
         <v>452</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I40" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="K40" s="10" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L40" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>74</v>
       </c>
@@ -25457,6 +25704,18 @@
       </c>
       <c r="C41" s="1" t="n">
         <v>965</v>
+      </c>
+      <c r="I41" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="J41" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="K41" s="17" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="L41" s="17" t="n">
+        <v>0.46</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
downloaded flux sus datasheets from drive for greyhound
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -1250,7 +1250,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1436,11 +1436,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="23223204"/>
-        <c:axId val="87622101"/>
+        <c:axId val="39196962"/>
+        <c:axId val="25460193"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="23223204"/>
+        <c:axId val="39196962"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1496,12 +1496,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87622101"/>
+        <c:crossAx val="25460193"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87622101"/>
+        <c:axId val="25460193"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1566,7 +1566,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23223204"/>
+        <c:crossAx val="39196962"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1614,7 +1614,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1812,11 +1812,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="5330152"/>
-        <c:axId val="62598404"/>
+        <c:axId val="95084969"/>
+        <c:axId val="45166253"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5330152"/>
+        <c:axId val="95084969"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1872,12 +1872,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62598404"/>
+        <c:crossAx val="45166253"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62598404"/>
+        <c:axId val="45166253"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1942,7 +1942,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5330152"/>
+        <c:crossAx val="95084969"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1990,7 +1990,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2176,11 +2176,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="19185146"/>
-        <c:axId val="59481067"/>
+        <c:axId val="10048094"/>
+        <c:axId val="14506287"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="19185146"/>
+        <c:axId val="10048094"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2236,12 +2236,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59481067"/>
+        <c:crossAx val="14506287"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59481067"/>
+        <c:axId val="14506287"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2306,7 +2306,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19185146"/>
+        <c:crossAx val="10048094"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2354,7 +2354,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2552,11 +2552,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="21913232"/>
-        <c:axId val="25867762"/>
+        <c:axId val="99092388"/>
+        <c:axId val="1446412"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="21913232"/>
+        <c:axId val="99092388"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2612,12 +2612,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25867762"/>
+        <c:crossAx val="1446412"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="25867762"/>
+        <c:axId val="1446412"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2682,7 +2682,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21913232"/>
+        <c:crossAx val="99092388"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2730,7 +2730,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3051,11 +3051,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="30388415"/>
-        <c:axId val="49200706"/>
+        <c:axId val="40947818"/>
+        <c:axId val="44510707"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30388415"/>
+        <c:axId val="40947818"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3111,12 +3111,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49200706"/>
+        <c:crossAx val="44510707"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49200706"/>
+        <c:axId val="44510707"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3172,7 +3172,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30388415"/>
+        <c:crossAx val="40947818"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3199,7 +3199,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3457,11 +3457,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="85715848"/>
-        <c:axId val="42577379"/>
+        <c:axId val="9516522"/>
+        <c:axId val="22655309"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85715848"/>
+        <c:axId val="9516522"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3517,12 +3517,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42577379"/>
+        <c:crossAx val="22655309"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42577379"/>
+        <c:axId val="22655309"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3578,7 +3578,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85715848"/>
+        <c:crossAx val="9516522"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3605,7 +3605,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3910,11 +3910,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="19328804"/>
-        <c:axId val="93182625"/>
+        <c:axId val="20189493"/>
+        <c:axId val="16709400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="19328804"/>
+        <c:axId val="20189493"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,12 +3970,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93182625"/>
+        <c:crossAx val="16709400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93182625"/>
+        <c:axId val="16709400"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4031,7 +4031,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19328804"/>
+        <c:crossAx val="20189493"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4058,7 +4058,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4391,11 +4391,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="6621348"/>
-        <c:axId val="60154432"/>
+        <c:axId val="85029569"/>
+        <c:axId val="88692116"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="6621348"/>
+        <c:axId val="85029569"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4451,12 +4451,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60154432"/>
+        <c:crossAx val="88692116"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60154432"/>
+        <c:axId val="88692116"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4512,7 +4512,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6621348"/>
+        <c:crossAx val="85029569"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4539,7 +4539,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4842,11 +4842,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="37765514"/>
-        <c:axId val="55431340"/>
+        <c:axId val="2580477"/>
+        <c:axId val="15565410"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37765514"/>
+        <c:axId val="2580477"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4902,12 +4902,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55431340"/>
+        <c:crossAx val="15565410"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55431340"/>
+        <c:axId val="15565410"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4963,7 +4963,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37765514"/>
+        <c:crossAx val="2580477"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4990,7 +4990,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5295,11 +5295,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="13490374"/>
-        <c:axId val="31700314"/>
+        <c:axId val="75191475"/>
+        <c:axId val="74614952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="13490374"/>
+        <c:axId val="75191475"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5355,12 +5355,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31700314"/>
+        <c:crossAx val="74614952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="31700314"/>
+        <c:axId val="74614952"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5416,7 +5416,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13490374"/>
+        <c:crossAx val="75191475"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5770,7 +5770,7 @@
   <dimension ref="A1:S70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="O23" activeCellId="0" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
saved 2017 fluxes with corrected flux vales
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -1250,7 +1250,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1436,11 +1436,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="39196962"/>
-        <c:axId val="25460193"/>
+        <c:axId val="41073200"/>
+        <c:axId val="68991048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39196962"/>
+        <c:axId val="41073200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1496,12 +1496,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25460193"/>
+        <c:crossAx val="68991048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="25460193"/>
+        <c:axId val="68991048"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1566,7 +1566,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39196962"/>
+        <c:crossAx val="41073200"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1614,7 +1614,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1812,11 +1812,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="95084969"/>
-        <c:axId val="45166253"/>
+        <c:axId val="51595607"/>
+        <c:axId val="87823734"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95084969"/>
+        <c:axId val="51595607"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1872,12 +1872,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45166253"/>
+        <c:crossAx val="87823734"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45166253"/>
+        <c:axId val="87823734"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1942,7 +1942,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95084969"/>
+        <c:crossAx val="51595607"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1990,7 +1990,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2176,11 +2176,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="10048094"/>
-        <c:axId val="14506287"/>
+        <c:axId val="73932651"/>
+        <c:axId val="38880092"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="10048094"/>
+        <c:axId val="73932651"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2236,12 +2236,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14506287"/>
+        <c:crossAx val="38880092"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14506287"/>
+        <c:axId val="38880092"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2306,7 +2306,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10048094"/>
+        <c:crossAx val="73932651"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2354,7 +2354,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2552,11 +2552,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="99092388"/>
-        <c:axId val="1446412"/>
+        <c:axId val="92790797"/>
+        <c:axId val="15325911"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99092388"/>
+        <c:axId val="92790797"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2612,12 +2612,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1446412"/>
+        <c:crossAx val="15325911"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1446412"/>
+        <c:axId val="15325911"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2682,7 +2682,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99092388"/>
+        <c:crossAx val="92790797"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2730,7 +2730,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3051,11 +3051,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="40947818"/>
-        <c:axId val="44510707"/>
+        <c:axId val="62348196"/>
+        <c:axId val="68300489"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40947818"/>
+        <c:axId val="62348196"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3111,12 +3111,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44510707"/>
+        <c:crossAx val="68300489"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44510707"/>
+        <c:axId val="68300489"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3172,7 +3172,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40947818"/>
+        <c:crossAx val="62348196"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3199,7 +3199,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3457,11 +3457,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="9516522"/>
-        <c:axId val="22655309"/>
+        <c:axId val="28739725"/>
+        <c:axId val="47662269"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9516522"/>
+        <c:axId val="28739725"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3517,12 +3517,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22655309"/>
+        <c:crossAx val="47662269"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="22655309"/>
+        <c:axId val="47662269"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3578,7 +3578,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9516522"/>
+        <c:crossAx val="28739725"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3605,7 +3605,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3910,11 +3910,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="20189493"/>
-        <c:axId val="16709400"/>
+        <c:axId val="31889755"/>
+        <c:axId val="11336594"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20189493"/>
+        <c:axId val="31889755"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,12 +3970,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16709400"/>
+        <c:crossAx val="11336594"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="16709400"/>
+        <c:axId val="11336594"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4031,7 +4031,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20189493"/>
+        <c:crossAx val="31889755"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4058,7 +4058,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4391,11 +4391,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="85029569"/>
-        <c:axId val="88692116"/>
+        <c:axId val="29035889"/>
+        <c:axId val="56678776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85029569"/>
+        <c:axId val="29035889"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4451,12 +4451,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88692116"/>
+        <c:crossAx val="56678776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88692116"/>
+        <c:axId val="56678776"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4512,7 +4512,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85029569"/>
+        <c:crossAx val="29035889"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4539,7 +4539,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4842,11 +4842,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2580477"/>
-        <c:axId val="15565410"/>
+        <c:axId val="49259597"/>
+        <c:axId val="46000355"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2580477"/>
+        <c:axId val="49259597"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4902,12 +4902,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15565410"/>
+        <c:crossAx val="46000355"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="15565410"/>
+        <c:axId val="46000355"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4963,7 +4963,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2580477"/>
+        <c:crossAx val="49259597"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4990,7 +4990,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5295,11 +5295,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="75191475"/>
-        <c:axId val="74614952"/>
+        <c:axId val="40182377"/>
+        <c:axId val="90033120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75191475"/>
+        <c:axId val="40182377"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5355,12 +5355,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74614952"/>
+        <c:crossAx val="90033120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74614952"/>
+        <c:axId val="90033120"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5416,7 +5416,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75191475"/>
+        <c:crossAx val="40182377"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>

<commit_message>
fixed annotations in stable isos plots all years
</commit_message>
<xml_diff>
--- a/data/flux/2017-fluxes.xlsx
+++ b/data/flux/2017-fluxes.xlsx
@@ -93,7 +93,7 @@
     <t xml:space="preserve">N/C</t>
   </si>
   <si>
-    <t xml:space="preserve">zoop_carcass flux  (umol C/m2/day)</t>
+    <t xml:space="preserve">zoop C (umol C/m2/day)</t>
   </si>
   <si>
     <t xml:space="preserve">1-1_60m_+p</t>
@@ -1274,7 +1274,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1460,11 +1460,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="97543105"/>
-        <c:axId val="99886828"/>
+        <c:axId val="77766753"/>
+        <c:axId val="98383535"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97543105"/>
+        <c:axId val="77766753"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1520,12 +1520,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99886828"/>
+        <c:crossAx val="98383535"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99886828"/>
+        <c:axId val="98383535"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1590,7 +1590,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97543105"/>
+        <c:crossAx val="77766753"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1638,7 +1638,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1836,11 +1836,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="64660023"/>
-        <c:axId val="94793259"/>
+        <c:axId val="44206508"/>
+        <c:axId val="28085196"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64660023"/>
+        <c:axId val="44206508"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1896,12 +1896,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94793259"/>
+        <c:crossAx val="28085196"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94793259"/>
+        <c:axId val="28085196"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1966,7 +1966,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64660023"/>
+        <c:crossAx val="44206508"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2014,7 +2014,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2200,11 +2200,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="25840924"/>
-        <c:axId val="16576114"/>
+        <c:axId val="85014572"/>
+        <c:axId val="37805369"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="25840924"/>
+        <c:axId val="85014572"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2260,12 +2260,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16576114"/>
+        <c:crossAx val="37805369"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="16576114"/>
+        <c:axId val="37805369"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2330,7 +2330,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25840924"/>
+        <c:crossAx val="85014572"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2378,7 +2378,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2576,11 +2576,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="82362321"/>
-        <c:axId val="53710788"/>
+        <c:axId val="59632276"/>
+        <c:axId val="24382993"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82362321"/>
+        <c:axId val="59632276"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2636,12 +2636,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53710788"/>
+        <c:crossAx val="24382993"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53710788"/>
+        <c:axId val="24382993"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2706,7 +2706,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82362321"/>
+        <c:crossAx val="59632276"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2754,7 +2754,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3075,11 +3075,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="56862092"/>
-        <c:axId val="90657406"/>
+        <c:axId val="16666532"/>
+        <c:axId val="2637307"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56862092"/>
+        <c:axId val="16666532"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3135,12 +3135,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90657406"/>
+        <c:crossAx val="2637307"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90657406"/>
+        <c:axId val="2637307"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3196,7 +3196,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56862092"/>
+        <c:crossAx val="16666532"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3223,7 +3223,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3481,11 +3481,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="69012214"/>
-        <c:axId val="2507348"/>
+        <c:axId val="63898970"/>
+        <c:axId val="27161815"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69012214"/>
+        <c:axId val="63898970"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3541,12 +3541,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2507348"/>
+        <c:crossAx val="27161815"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2507348"/>
+        <c:axId val="27161815"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3602,7 +3602,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69012214"/>
+        <c:crossAx val="63898970"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3629,7 +3629,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3934,11 +3934,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="37480822"/>
-        <c:axId val="27149654"/>
+        <c:axId val="20839539"/>
+        <c:axId val="83658289"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37480822"/>
+        <c:axId val="20839539"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3994,12 +3994,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27149654"/>
+        <c:crossAx val="83658289"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="27149654"/>
+        <c:axId val="83658289"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4055,7 +4055,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37480822"/>
+        <c:crossAx val="20839539"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4082,7 +4082,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4415,11 +4415,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="78054356"/>
-        <c:axId val="82986471"/>
+        <c:axId val="77489383"/>
+        <c:axId val="7061333"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="78054356"/>
+        <c:axId val="77489383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4475,12 +4475,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82986471"/>
+        <c:crossAx val="7061333"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82986471"/>
+        <c:axId val="7061333"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4536,7 +4536,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78054356"/>
+        <c:crossAx val="77489383"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4563,7 +4563,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4866,11 +4866,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48449765"/>
-        <c:axId val="12668979"/>
+        <c:axId val="48645548"/>
+        <c:axId val="2189125"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48449765"/>
+        <c:axId val="48645548"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4926,12 +4926,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12668979"/>
+        <c:crossAx val="2189125"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="12668979"/>
+        <c:axId val="2189125"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4987,7 +4987,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48449765"/>
+        <c:crossAx val="48645548"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5014,7 +5014,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5319,11 +5319,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="11927045"/>
-        <c:axId val="79952463"/>
+        <c:axId val="22776420"/>
+        <c:axId val="15816041"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="11927045"/>
+        <c:axId val="22776420"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5379,12 +5379,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79952463"/>
+        <c:crossAx val="15816041"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79952463"/>
+        <c:axId val="15816041"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5440,7 +5440,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11927045"/>
+        <c:crossAx val="22776420"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5794,7 +5794,7 @@
   <dimension ref="A1:V70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8494,7 +8494,7 @@
   <dimension ref="A1:C954"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="T38" activeCellId="0" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13587,7 +13587,7 @@
   <dimension ref="A1:BJ70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24932,8 +24932,8 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25145,8 +25145,8 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T25" activeCellId="0" sqref="T25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25717,8 +25717,8 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>